<commit_message>
Umfrage Auswertung Dienstkategorien und Dienstaufteilung
</commit_message>
<xml_diff>
--- a/Umfrage/Auswertung.xlsx
+++ b/Umfrage/Auswertung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>Team Collaboration</t>
   </si>
   <si>
-    <t>Messaging-Service</t>
-  </si>
-  <si>
     <t>Sonstige</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>Wirtschaftsinformatik</t>
+  </si>
+  <si>
+    <t>Instant-Messaging</t>
   </si>
 </sst>
 </file>
@@ -2322,7 +2322,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1">
+                  <a:rPr lang="de-DE" sz="1100" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3110,7 +3110,7 @@
                   <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:rPr lang="de-DE" sz="1600" b="0"/>
                   <a:t>Web-Dienst</a:t>
                 </a:r>
               </a:p>
@@ -3156,8 +3156,8 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1600"/>
-                  <a:t>Anzahl Nutzer</a:t>
+                  <a:rPr lang="de-DE" sz="1600" b="0"/>
+                  <a:t>Anzahl Nutzer in %</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3345,43 +3345,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Dienstkategorien</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -3524,7 +3488,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3539,7 +3503,6 @@
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="bestFit"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -3579,7 +3542,7 @@
                   <c:v>Cloud-Storage</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Messaging-Service</c:v>
+                  <c:v>Instant-Messaging</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Versionsverwaltung</c:v>
@@ -3627,7 +3590,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -3662,7 +3624,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4922,8 +4884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO538"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5038,7 +5000,7 @@
         <v>81</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>66</v>
@@ -5317,7 +5279,7 @@
         <v>0.92</v>
       </c>
       <c r="Q4" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P4&gt;0.7,"A",IF(P4&gt;0.1,"B","C"))</f>
         <v>A</v>
       </c>
       <c r="R4" s="1">
@@ -5325,15 +5287,15 @@
         <v>220</v>
       </c>
       <c r="S4" s="1">
-        <f t="shared" ref="S4:S26" si="6">R4/O4</f>
+        <f>R4/O4</f>
         <v>2.3913043478260869</v>
       </c>
       <c r="T4" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S4-1)/4)</f>
         <v>0.65217391304347827</v>
       </c>
       <c r="U4" s="3">
-        <f t="shared" si="3"/>
+        <f>(P4+T4+Z4)/3</f>
         <v>0.67623188405797097</v>
       </c>
       <c r="V4" s="9">
@@ -5349,11 +5311,11 @@
         <v>0.33695652173913043</v>
       </c>
       <c r="Y4" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E4:E1002,D4:D1002,M4)/O4</f>
         <v>2.0869565217391304</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y4-1)/2)</f>
         <v>0.45652173913043481</v>
       </c>
       <c r="AA4" s="9">
@@ -5455,10 +5417,10 @@
         <v>15</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" ref="O5:O26" si="7">COUNTIF(D6:D1004,M5)</f>
+        <f>COUNTIF(D6:D1004,M5)</f>
         <v>79</v>
       </c>
       <c r="P5" s="3">
@@ -5466,103 +5428,103 @@
         <v>0.79</v>
       </c>
       <c r="Q5" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P5&gt;0.7,"A",IF(P5&gt;0.1,"B","C"))</f>
         <v>A</v>
       </c>
       <c r="R5" s="1">
-        <f t="shared" ref="R5:R26" si="8">SUMIFS(F6:F1004,D6:D1004,M5)</f>
+        <f>SUMIFS(F6:F1004,D6:D1004,M5)</f>
         <v>153</v>
       </c>
       <c r="S5" s="1">
-        <f t="shared" si="6"/>
+        <f>R5/O5</f>
         <v>1.9367088607594938</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S5-1)/4)</f>
         <v>0.76582278481012656</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" si="3"/>
+        <f>(P5+T5+Z5)/3</f>
         <v>0.84561181434599153</v>
       </c>
       <c r="V5" s="9">
-        <f t="shared" ref="V5:V26" si="9">COUNTIFS(D5:D1003,M5,E5:E1003,"1")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,E5:E1003,"1")/O5</f>
         <v>0.96202531645569622</v>
       </c>
       <c r="W5" s="3">
-        <f t="shared" ref="W5:W26" si="10">COUNTIFS(D5:D1003,M5,E5:E1003,"2")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,E5:E1003,"2")/O5</f>
         <v>3.7974683544303799E-2</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" ref="X5:X26" si="11">COUNTIFS(D5:D1003,M5,E5:E1003,"3")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,E5:E1003,"3")/O5</f>
         <v>0</v>
       </c>
       <c r="Y5" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E5:E1003,D5:D1003,M5)/O5</f>
         <v>1.0379746835443038</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y5-1)/2)</f>
         <v>0.98101265822784811</v>
       </c>
       <c r="AA5" s="9">
-        <f t="shared" ref="AA5:AA26" si="12">COUNTIFS(D5:D1003,M5,G5:G1003,"1")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,G5:G1003,"1")/O5</f>
         <v>0</v>
       </c>
       <c r="AB5" s="3">
-        <f t="shared" ref="AB5:AB26" si="13">COUNTIFS(D5:D1003,M5,G5:G1003,"2")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,G5:G1003,"2")/O5</f>
         <v>7.5949367088607597E-2</v>
       </c>
       <c r="AC5" s="3">
-        <f t="shared" ref="AC5:AC26" si="14">COUNTIFS(D5:D1003,M5,G5:G1003,"3")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,G5:G1003,"3")/O5</f>
         <v>0.810126582278481</v>
       </c>
       <c r="AD5" s="9">
-        <f t="shared" ref="AD5:AD26" si="15">(COUNTIFS(D6:D1003,M5,H6:H1003,"1")+COUNTIFS(D6:D1003,M5,H6:H1003,"1,2"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,H6:H1003,"1")+COUNTIFS(D6:D1003,M5,H6:H1003,"1,2"))/O5</f>
         <v>0.379746835443038</v>
       </c>
       <c r="AE5" s="3">
-        <f t="shared" ref="AE5:AE26" si="16">(COUNTIFS(D6:D1003,M5,H6:H1003,"2")+COUNTIFS(D6:D1003,M5,H6:H1003,"1,2"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,H6:H1003,"2")+COUNTIFS(D6:D1003,M5,H6:H1003,"1,2"))/O5</f>
         <v>0.98734177215189878</v>
       </c>
       <c r="AF5" s="9">
-        <f t="shared" ref="AF5:AF26" si="17">(COUNTIFS(D6:D1003,M5,I6:I1003,"1")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2,3"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,I6:I1003,"1")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2,3"))/O5</f>
         <v>0.29113924050632911</v>
       </c>
       <c r="AG5" s="3">
-        <f t="shared" ref="AG5:AG26" si="18">(COUNTIFS(D6:D1003,M5,I6:I1003,"2")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2")+COUNTIFS(D6:D1003,M5,I6:I1003,"2,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2,3"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,I6:I1003,"2")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2")+COUNTIFS(D6:D1003,M5,I6:I1003,"2,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2,3"))/O5</f>
         <v>0.31645569620253167</v>
       </c>
       <c r="AH5" s="3">
-        <f t="shared" ref="AH5:AH26" si="19">(COUNTIFS(D6:D1003,M5,I6:I1003,"3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"2,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2,3"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,I6:I1003,"3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"2,3")+COUNTIFS(D6:D1003,M5,I6:I1003,"1,2,3"))/O5</f>
         <v>0.93670886075949367</v>
       </c>
       <c r="AI5" s="9">
-        <f t="shared" ref="AI5:AI26" si="20">(COUNTIFS(D6:D1003,M5,J6:J1003,"1")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2,3"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,J6:J1003,"1")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2,3"))/O5</f>
         <v>0.73417721518987344</v>
       </c>
       <c r="AJ5" s="3">
-        <f t="shared" ref="AJ5:AJ26" si="21">(COUNTIFS(D6:D1003,M5,J6:J1003,"2")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2")+COUNTIFS(D6:D1003,M5,J6:J1003,"2,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2,3"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,J6:J1003,"2")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2")+COUNTIFS(D6:D1003,M5,J6:J1003,"2,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2,3"))/O5</f>
         <v>0.25316455696202533</v>
       </c>
       <c r="AK5" s="3">
-        <f t="shared" ref="AK5:AK26" si="22">(COUNTIFS(D6:D1003,M5,J6:J1003,"3+X3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"2,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2,3"))/O5</f>
+        <f>(COUNTIFS(D6:D1003,M5,J6:J1003,"3+X3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"2,3")+COUNTIFS(D6:D1003,M5,J6:J1003,"1,2,3"))/O5</f>
         <v>0.70886075949367089</v>
       </c>
       <c r="AL5" s="9">
-        <f t="shared" ref="AL5:AL26" si="23">COUNTIFS(D5:D1003,M5,K5:K1003,"1")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,K5:K1003,"1")/O5</f>
         <v>0.73417721518987344</v>
       </c>
       <c r="AM5" s="3">
-        <f t="shared" ref="AM5:AM26" si="24">COUNTIFS(D5:D1003,M5,K5:K1003,"2")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,K5:K1003,"2")/O5</f>
         <v>0.12658227848101267</v>
       </c>
       <c r="AN5" s="3">
-        <f t="shared" ref="AN5:AN26" si="25">COUNTIFS(D5:D1003,M5,K5:K1003,"3")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,K5:K1003,"3")/O5</f>
         <v>0</v>
       </c>
       <c r="AO5" s="3">
-        <f t="shared" ref="AO5:AO26" si="26">COUNTIFS(D5:D1003,M5,K5:K1003,"4")/O5</f>
+        <f>COUNTIFS(D5:D1003,M5,K5:K1003,"4")/O5</f>
         <v>0.13924050632911392</v>
       </c>
     </row>
@@ -5607,111 +5569,111 @@
         <v>82</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D7:D1005,M6)</f>
         <v>57</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" ref="P6:P26" si="27">O6/$M$32</f>
+        <f>O6/$M$32</f>
         <v>0.56999999999999995</v>
       </c>
       <c r="Q6" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P6&gt;0.7,"A",IF(P6&gt;0.1,"B","C"))</f>
         <v>B</v>
       </c>
       <c r="R6" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F7:F1005,D7:D1005,M6)</f>
         <v>100</v>
       </c>
       <c r="S6" s="1">
-        <f t="shared" si="6"/>
+        <f>R6/O6</f>
         <v>1.7543859649122806</v>
       </c>
       <c r="T6" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S6-1)/4)</f>
         <v>0.81140350877192979</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" si="3"/>
+        <f>(P6+T6+Z6)/3</f>
         <v>0.66807017543859637</v>
       </c>
       <c r="V6" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D6:D1004,M6,E6:E1004,"1")/O6</f>
         <v>0.42105263157894735</v>
       </c>
       <c r="W6" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D6:D1004,M6,E6:E1004,"2")/O6</f>
         <v>0.40350877192982454</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D6:D1004,M6,E6:E1004,"3")/O6</f>
         <v>0.17543859649122806</v>
       </c>
       <c r="Y6" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E6:E1004,D6:D1004,M6)/O6</f>
         <v>1.7543859649122806</v>
       </c>
       <c r="Z6" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y6-1)/2)</f>
         <v>0.6228070175438597</v>
       </c>
       <c r="AA6" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D6:D1004,M6,G6:G1004,"1")/O6</f>
         <v>0</v>
       </c>
       <c r="AB6" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D6:D1004,M6,G6:G1004,"2")/O6</f>
         <v>0.21052631578947367</v>
       </c>
       <c r="AC6" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D6:D1004,M6,G6:G1004,"3")/O6</f>
         <v>0.70175438596491224</v>
       </c>
       <c r="AD6" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D7:D1004,M6,H7:H1004,"1")+COUNTIFS(D7:D1004,M6,H7:H1004,"1,2"))/O6</f>
         <v>0.98245614035087714</v>
       </c>
       <c r="AE6" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D7:D1004,M6,H7:H1004,"2")+COUNTIFS(D7:D1004,M6,H7:H1004,"1,2"))/O6</f>
         <v>0.68421052631578949</v>
       </c>
       <c r="AF6" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D7:D1004,M6,I7:I1004,"1")+COUNTIFS(D7:D1004,M6,I7:I1004,"1,2")+COUNTIFS(D7:D1004,M6,I7:I1004,"1,3")+COUNTIFS(D7:D1004,M6,I7:I1004,"1,2,3"))/O6</f>
         <v>0.68421052631578949</v>
       </c>
       <c r="AG6" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D7:D1004,M6,I7:I1004,"2")+COUNTIFS(D7:D1004,M6,I7:I1004,"1,2")+COUNTIFS(D7:D1004,M6,I7:I1004,"2,3")+COUNTIFS(D7:D1004,M6,I7:I1004,"1,2,3"))/O6</f>
         <v>0.77192982456140347</v>
       </c>
       <c r="AH6" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D7:D1004,M6,I7:I1004,"3")+COUNTIFS(D7:D1004,M6,I7:I1004,"1,3")+COUNTIFS(D7:D1004,M6,I7:I1004,"2,3")+COUNTIFS(D7:D1004,M6,I7:I1004,"1,2,3"))/O6</f>
         <v>0.61403508771929827</v>
       </c>
       <c r="AI6" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D7:D1004,M6,J7:J1004,"1")+COUNTIFS(D7:D1004,M6,J7:J1004,"1,2")+COUNTIFS(D7:D1004,M6,J7:J1004,"1,3")+COUNTIFS(D7:D1004,M6,J7:J1004,"1,2,3"))/O6</f>
         <v>0.75438596491228072</v>
       </c>
       <c r="AJ6" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D7:D1004,M6,J7:J1004,"2")+COUNTIFS(D7:D1004,M6,J7:J1004,"1,2")+COUNTIFS(D7:D1004,M6,J7:J1004,"2,3")+COUNTIFS(D7:D1004,M6,J7:J1004,"1,2,3"))/O6</f>
         <v>0.12280701754385964</v>
       </c>
       <c r="AK6" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D7:D1004,M6,J7:J1004,"3+X3")+COUNTIFS(D7:D1004,M6,J7:J1004,"1,3")+COUNTIFS(D7:D1004,M6,J7:J1004,"2,3")+COUNTIFS(D7:D1004,M6,J7:J1004,"1,2,3"))/O6</f>
         <v>0.59649122807017541</v>
       </c>
       <c r="AL6" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D6:D1004,M6,K6:K1004,"1")/O6</f>
         <v>0.61403508771929827</v>
       </c>
       <c r="AM6" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D6:D1004,M6,K6:K1004,"2")/O6</f>
         <v>0.24561403508771928</v>
       </c>
       <c r="AN6" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D6:D1004,M6,K6:K1004,"3")/O6</f>
         <v>0</v>
       </c>
       <c r="AO6" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D6:D1004,M6,K6:K1004,"4")/O6</f>
         <v>0.14035087719298245</v>
       </c>
     </row>
@@ -5753,114 +5715,114 @@
         <v>18</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D8:D1006,M7)</f>
         <v>39</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="27"/>
+        <f>O7/$M$32</f>
         <v>0.39</v>
       </c>
       <c r="Q7" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P7&gt;0.7,"A",IF(P7&gt;0.1,"B","C"))</f>
         <v>B</v>
       </c>
       <c r="R7" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F8:F1006,D8:D1006,M7)</f>
         <v>82</v>
       </c>
       <c r="S7" s="1">
-        <f t="shared" si="6"/>
+        <f>R7/O7</f>
         <v>2.1025641025641026</v>
       </c>
       <c r="T7" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S7-1)/4)</f>
         <v>0.72435897435897434</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" si="3"/>
+        <f>(P7+T7+Z7)/3</f>
         <v>0.52529914529914523</v>
       </c>
       <c r="V7" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D7:D1005,M7,E7:E1005,"1")/O7</f>
         <v>0.25641025641025639</v>
       </c>
       <c r="W7" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D7:D1005,M7,E7:E1005,"2")/O7</f>
         <v>0.41025641025641024</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D7:D1005,M7,E7:E1005,"3")/O7</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="Y7" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E7:E1005,D7:D1005,M7)/O7</f>
         <v>2.0769230769230771</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y7-1)/2)</f>
         <v>0.46153846153846145</v>
       </c>
       <c r="AA7" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D7:D1005,M7,G7:G1005,"1")/O7</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="AB7" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D7:D1005,M7,G7:G1005,"2")/O7</f>
         <v>0.4358974358974359</v>
       </c>
       <c r="AC7" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D7:D1005,M7,G7:G1005,"3")/O7</f>
         <v>0.38461538461538464</v>
       </c>
       <c r="AD7" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D8:D1005,M7,H8:H1005,"1")+COUNTIFS(D8:D1005,M7,H8:H1005,"1,2"))/O7</f>
         <v>1</v>
       </c>
       <c r="AE7" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D8:D1005,M7,H8:H1005,"2")+COUNTIFS(D8:D1005,M7,H8:H1005,"1,2"))/O7</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="AF7" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D8:D1005,M7,I8:I1005,"1")+COUNTIFS(D8:D1005,M7,I8:I1005,"1,2")+COUNTIFS(D8:D1005,M7,I8:I1005,"1,3")+COUNTIFS(D8:D1005,M7,I8:I1005,"1,2,3"))/O7</f>
         <v>0.58974358974358976</v>
       </c>
       <c r="AG7" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D8:D1005,M7,I8:I1005,"2")+COUNTIFS(D8:D1005,M7,I8:I1005,"1,2")+COUNTIFS(D8:D1005,M7,I8:I1005,"2,3")+COUNTIFS(D8:D1005,M7,I8:I1005,"1,2,3"))/O7</f>
         <v>0.82051282051282048</v>
       </c>
       <c r="AH7" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D8:D1005,M7,I8:I1005,"3")+COUNTIFS(D8:D1005,M7,I8:I1005,"1,3")+COUNTIFS(D8:D1005,M7,I8:I1005,"2,3")+COUNTIFS(D8:D1005,M7,I8:I1005,"1,2,3"))/O7</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="AI7" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D8:D1005,M7,J8:J1005,"1")+COUNTIFS(D8:D1005,M7,J8:J1005,"1,2")+COUNTIFS(D8:D1005,M7,J8:J1005,"1,3")+COUNTIFS(D8:D1005,M7,J8:J1005,"1,2,3"))/O7</f>
         <v>0.94871794871794868</v>
       </c>
       <c r="AJ7" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D8:D1005,M7,J8:J1005,"2")+COUNTIFS(D8:D1005,M7,J8:J1005,"1,2")+COUNTIFS(D8:D1005,M7,J8:J1005,"2,3")+COUNTIFS(D8:D1005,M7,J8:J1005,"1,2,3"))/O7</f>
         <v>0.23076923076923078</v>
       </c>
       <c r="AK7" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D8:D1005,M7,J8:J1005,"3+X3")+COUNTIFS(D8:D1005,M7,J8:J1005,"1,3")+COUNTIFS(D8:D1005,M7,J8:J1005,"2,3")+COUNTIFS(D8:D1005,M7,J8:J1005,"1,2,3"))/O7</f>
         <v>0.46153846153846156</v>
       </c>
       <c r="AL7" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D7:D1005,M7,K7:K1005,"1")/O7</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AM7" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D7:D1005,M7,K7:K1005,"2")/O7</f>
         <v>0.35897435897435898</v>
       </c>
       <c r="AN7" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D7:D1005,M7,K7:K1005,"3")/O7</f>
         <v>0.10256410256410256</v>
       </c>
       <c r="AO7" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D7:D1005,M7,K7:K1005,"4")/O7</f>
         <v>0.20512820512820512</v>
       </c>
     </row>
@@ -5902,114 +5864,114 @@
         <v>19</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D9:D1007,M8)</f>
         <v>29</v>
       </c>
       <c r="P8" s="3">
-        <f t="shared" si="27"/>
+        <f>O8/$M$32</f>
         <v>0.28999999999999998</v>
       </c>
       <c r="Q8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P8&gt;0.7,"A",IF(P8&gt;0.1,"B","C"))</f>
         <v>B</v>
       </c>
       <c r="R8" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F9:F1007,D9:D1007,M8)</f>
         <v>62</v>
       </c>
       <c r="S8" s="1">
-        <f t="shared" si="6"/>
+        <f>R8/O8</f>
         <v>2.1379310344827585</v>
       </c>
       <c r="T8" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S8-1)/4)</f>
         <v>0.71551724137931039</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" si="3"/>
+        <f>(P8+T8+Z8)/3</f>
         <v>0.45586206896551723</v>
       </c>
       <c r="V8" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D8:D1006,M8,E8:E1006,"1")/O8</f>
         <v>0.17241379310344829</v>
       </c>
       <c r="W8" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D8:D1006,M8,E8:E1006,"2")/O8</f>
         <v>0.37931034482758619</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D8:D1006,M8,E8:E1006,"3")/O8</f>
         <v>0.44827586206896552</v>
       </c>
       <c r="Y8" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E8:E1006,D8:D1006,M8)/O8</f>
         <v>2.2758620689655173</v>
       </c>
       <c r="Z8" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y8-1)/2)</f>
         <v>0.36206896551724133</v>
       </c>
       <c r="AA8" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D8:D1006,M8,G8:G1006,"1")/O8</f>
         <v>3.4482758620689655E-2</v>
       </c>
       <c r="AB8" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D8:D1006,M8,G8:G1006,"2")/O8</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="AC8" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D8:D1006,M8,G8:G1006,"3")/O8</f>
         <v>0.34482758620689657</v>
       </c>
       <c r="AD8" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D9:D1006,M8,H9:H1006,"1")+COUNTIFS(D9:D1006,M8,H9:H1006,"1,2"))/O8</f>
         <v>0.96551724137931039</v>
       </c>
       <c r="AE8" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D9:D1006,M8,H9:H1006,"2")+COUNTIFS(D9:D1006,M8,H9:H1006,"1,2"))/O8</f>
         <v>0.2413793103448276</v>
       </c>
       <c r="AF8" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D9:D1006,M8,I9:I1006,"1")+COUNTIFS(D9:D1006,M8,I9:I1006,"1,2")+COUNTIFS(D9:D1006,M8,I9:I1006,"1,3")+COUNTIFS(D9:D1006,M8,I9:I1006,"1,2,3"))/O8</f>
         <v>3.4482758620689655E-2</v>
       </c>
       <c r="AG8" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D9:D1006,M8,I9:I1006,"2")+COUNTIFS(D9:D1006,M8,I9:I1006,"1,2")+COUNTIFS(D9:D1006,M8,I9:I1006,"2,3")+COUNTIFS(D9:D1006,M8,I9:I1006,"1,2,3"))/O8</f>
         <v>1</v>
       </c>
       <c r="AH8" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D9:D1006,M8,I9:I1006,"3")+COUNTIFS(D9:D1006,M8,I9:I1006,"1,3")+COUNTIFS(D9:D1006,M8,I9:I1006,"2,3")+COUNTIFS(D9:D1006,M8,I9:I1006,"1,2,3"))/O8</f>
         <v>0.17241379310344829</v>
       </c>
       <c r="AI8" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D9:D1006,M8,J9:J1006,"1")+COUNTIFS(D9:D1006,M8,J9:J1006,"1,2")+COUNTIFS(D9:D1006,M8,J9:J1006,"1,3")+COUNTIFS(D9:D1006,M8,J9:J1006,"1,2,3"))/O8</f>
         <v>0.89655172413793105</v>
       </c>
       <c r="AJ8" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D9:D1006,M8,J9:J1006,"2")+COUNTIFS(D9:D1006,M8,J9:J1006,"1,2")+COUNTIFS(D9:D1006,M8,J9:J1006,"2,3")+COUNTIFS(D9:D1006,M8,J9:J1006,"1,2,3"))/O8</f>
         <v>0.13793103448275862</v>
       </c>
       <c r="AK8" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D9:D1006,M8,J9:J1006,"3+X3")+COUNTIFS(D9:D1006,M8,J9:J1006,"1,3")+COUNTIFS(D9:D1006,M8,J9:J1006,"2,3")+COUNTIFS(D9:D1006,M8,J9:J1006,"1,2,3"))/O8</f>
         <v>0.44827586206896552</v>
       </c>
       <c r="AL8" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D8:D1006,M8,K8:K1006,"1")/O8</f>
         <v>0.31034482758620691</v>
       </c>
       <c r="AM8" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D8:D1006,M8,K8:K1006,"2")/O8</f>
         <v>0.34482758620689657</v>
       </c>
       <c r="AN8" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D8:D1006,M8,K8:K1006,"3")/O8</f>
         <v>0.10344827586206896</v>
       </c>
       <c r="AO8" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D8:D1006,M8,K8:K1006,"4")/O8</f>
         <v>0.2413793103448276</v>
       </c>
     </row>
@@ -6051,114 +6013,114 @@
         <v>22</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D10:D1008,M9)</f>
         <v>28</v>
       </c>
       <c r="P9" s="3">
-        <f t="shared" si="27"/>
+        <f>O9/$M$32</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="Q9" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P9&gt;0.7,"A",IF(P9&gt;0.1,"B","C"))</f>
         <v>B</v>
       </c>
       <c r="R9" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F10:F1008,D10:D1008,M9)</f>
         <v>56</v>
       </c>
       <c r="S9" s="1">
-        <f t="shared" si="6"/>
+        <f>R9/O9</f>
         <v>2</v>
       </c>
       <c r="T9" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S9-1)/4)</f>
         <v>0.75</v>
       </c>
       <c r="U9" s="3">
-        <f t="shared" si="3"/>
+        <f>(P9+T9+Z9)/3</f>
         <v>0.56357142857142861</v>
       </c>
       <c r="V9" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D9:D1007,M9,E9:E1007,"1")/O9</f>
         <v>0.39285714285714285</v>
       </c>
       <c r="W9" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D9:D1007,M9,E9:E1007,"2")/O9</f>
         <v>0.5357142857142857</v>
       </c>
       <c r="X9" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D9:D1007,M9,E9:E1007,"3")/O9</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="Y9" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E9:E1007,D9:D1007,M9)/O9</f>
         <v>1.6785714285714286</v>
       </c>
       <c r="Z9" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y9-1)/2)</f>
         <v>0.6607142857142857</v>
       </c>
       <c r="AA9" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D9:D1007,M9,G9:G1007,"1")/O9</f>
         <v>0.32142857142857145</v>
       </c>
       <c r="AB9" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D9:D1007,M9,G9:G1007,"2")/O9</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="AC9" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D9:D1007,M9,G9:G1007,"3")/O9</f>
         <v>0.32142857142857145</v>
       </c>
       <c r="AD9" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D10:D1007,M9,H10:H1007,"1")+COUNTIFS(D10:D1007,M9,H10:H1007,"1,2"))/O9</f>
         <v>1</v>
       </c>
       <c r="AE9" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D10:D1007,M9,H10:H1007,"2")+COUNTIFS(D10:D1007,M9,H10:H1007,"1,2"))/O9</f>
         <v>0.10714285714285714</v>
       </c>
       <c r="AF9" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D10:D1007,M9,I10:I1007,"1")+COUNTIFS(D10:D1007,M9,I10:I1007,"1,2")+COUNTIFS(D10:D1007,M9,I10:I1007,"1,3")+COUNTIFS(D10:D1007,M9,I10:I1007,"1,2,3"))/O9</f>
         <v>0.35714285714285715</v>
       </c>
       <c r="AG9" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D10:D1007,M9,I10:I1007,"2")+COUNTIFS(D10:D1007,M9,I10:I1007,"1,2")+COUNTIFS(D10:D1007,M9,I10:I1007,"2,3")+COUNTIFS(D10:D1007,M9,I10:I1007,"1,2,3"))/O9</f>
         <v>0.9642857142857143</v>
       </c>
       <c r="AH9" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D10:D1007,M9,I10:I1007,"3")+COUNTIFS(D10:D1007,M9,I10:I1007,"1,3")+COUNTIFS(D10:D1007,M9,I10:I1007,"2,3")+COUNTIFS(D10:D1007,M9,I10:I1007,"1,2,3"))/O9</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="AI9" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D10:D1007,M9,J10:J1007,"1")+COUNTIFS(D10:D1007,M9,J10:J1007,"1,2")+COUNTIFS(D10:D1007,M9,J10:J1007,"1,3")+COUNTIFS(D10:D1007,M9,J10:J1007,"1,2,3"))/O9</f>
         <v>0.9642857142857143</v>
       </c>
       <c r="AJ9" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D10:D1007,M9,J10:J1007,"2")+COUNTIFS(D10:D1007,M9,J10:J1007,"1,2")+COUNTIFS(D10:D1007,M9,J10:J1007,"2,3")+COUNTIFS(D10:D1007,M9,J10:J1007,"1,2,3"))/O9</f>
         <v>0.10714285714285714</v>
       </c>
       <c r="AK9" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D10:D1007,M9,J10:J1007,"3+X3")+COUNTIFS(D10:D1007,M9,J10:J1007,"1,3")+COUNTIFS(D10:D1007,M9,J10:J1007,"2,3")+COUNTIFS(D10:D1007,M9,J10:J1007,"1,2,3"))/O9</f>
         <v>0.35714285714285715</v>
       </c>
       <c r="AL9" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D9:D1007,M9,K9:K1007,"1")/O9</f>
         <v>0.5</v>
       </c>
       <c r="AM9" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D9:D1007,M9,K9:K1007,"2")/O9</f>
         <v>0.32142857142857145</v>
       </c>
       <c r="AN9" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D9:D1007,M9,K9:K1007,"3")/O9</f>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="AO9" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D9:D1007,M9,K9:K1007,"4")/O9</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -6200,114 +6162,114 @@
         <v>31</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D11:D1009,M10)</f>
         <v>27</v>
       </c>
       <c r="P10" s="3">
-        <f t="shared" si="27"/>
+        <f>O10/$M$32</f>
         <v>0.27</v>
       </c>
       <c r="Q10" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P10&gt;0.7,"A",IF(P10&gt;0.1,"B","C"))</f>
         <v>B</v>
       </c>
       <c r="R10" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F11:F1009,D11:D1009,M10)</f>
         <v>54</v>
       </c>
       <c r="S10" s="1">
-        <f t="shared" si="6"/>
+        <f>R10/O10</f>
         <v>2</v>
       </c>
       <c r="T10" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S10-1)/4)</f>
         <v>0.75</v>
       </c>
       <c r="U10" s="3">
-        <f t="shared" si="3"/>
+        <f>(P10+T10+Z10)/3</f>
         <v>0.5251851851851852</v>
       </c>
       <c r="V10" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D10:D1008,M10,E10:E1008,"1")/O10</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="W10" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D10:D1008,M10,E10:E1008,"2")/O10</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="X10" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D10:D1008,M10,E10:E1008,"3")/O10</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="Y10" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E10:E1008,D10:D1008,M10)/O10</f>
         <v>1.8888888888888888</v>
       </c>
       <c r="Z10" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y10-1)/2)</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="AA10" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D10:D1008,M10,G10:G1008,"1")/O10</f>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="AB10" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D10:D1008,M10,G10:G1008,"2")/O10</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AC10" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D10:D1008,M10,G10:G1008,"3")/O10</f>
         <v>0.18518518518518517</v>
       </c>
       <c r="AD10" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D11:D1008,M10,H11:H1008,"1")+COUNTIFS(D11:D1008,M10,H11:H1008,"1,2"))/O10</f>
         <v>0.92592592592592593</v>
       </c>
       <c r="AE10" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D11:D1008,M10,H11:H1008,"2")+COUNTIFS(D11:D1008,M10,H11:H1008,"1,2"))/O10</f>
         <v>0.7407407407407407</v>
       </c>
       <c r="AF10" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D11:D1008,M10,I11:I1008,"1")+COUNTIFS(D11:D1008,M10,I11:I1008,"1,2")+COUNTIFS(D11:D1008,M10,I11:I1008,"1,3")+COUNTIFS(D11:D1008,M10,I11:I1008,"1,2,3"))/O10</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="AG10" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D11:D1008,M10,I11:I1008,"2")+COUNTIFS(D11:D1008,M10,I11:I1008,"1,2")+COUNTIFS(D11:D1008,M10,I11:I1008,"2,3")+COUNTIFS(D11:D1008,M10,I11:I1008,"1,2,3"))/O10</f>
         <v>0.70370370370370372</v>
       </c>
       <c r="AH10" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D11:D1008,M10,I11:I1008,"3")+COUNTIFS(D11:D1008,M10,I11:I1008,"1,3")+COUNTIFS(D11:D1008,M10,I11:I1008,"2,3")+COUNTIFS(D11:D1008,M10,I11:I1008,"1,2,3"))/O10</f>
         <v>0.70370370370370372</v>
       </c>
       <c r="AI10" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D11:D1008,M10,J11:J1008,"1")+COUNTIFS(D11:D1008,M10,J11:J1008,"1,2")+COUNTIFS(D11:D1008,M10,J11:J1008,"1,3")+COUNTIFS(D11:D1008,M10,J11:J1008,"1,2,3"))/O10</f>
         <v>1</v>
       </c>
       <c r="AJ10" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D11:D1008,M10,J11:J1008,"2")+COUNTIFS(D11:D1008,M10,J11:J1008,"1,2")+COUNTIFS(D11:D1008,M10,J11:J1008,"2,3")+COUNTIFS(D11:D1008,M10,J11:J1008,"1,2,3"))/O10</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="AK10" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D11:D1008,M10,J11:J1008,"3+X3")+COUNTIFS(D11:D1008,M10,J11:J1008,"1,3")+COUNTIFS(D11:D1008,M10,J11:J1008,"2,3")+COUNTIFS(D11:D1008,M10,J11:J1008,"1,2,3"))/O10</f>
         <v>0.29629629629629628</v>
       </c>
       <c r="AL10" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D10:D1008,M10,K10:K1008,"1")/O10</f>
         <v>0.40740740740740738</v>
       </c>
       <c r="AM10" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D10:D1008,M10,K10:K1008,"2")/O10</f>
         <v>0.40740740740740738</v>
       </c>
       <c r="AN10" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D10:D1008,M10,K10:K1008,"3")/O10</f>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="AO10" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D10:D1008,M10,K10:K1008,"4")/O10</f>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -6349,114 +6311,114 @@
         <v>17</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D12:D1010,M11)</f>
         <v>26</v>
       </c>
       <c r="P11" s="3">
-        <f t="shared" si="27"/>
+        <f>O11/$M$32</f>
         <v>0.26</v>
       </c>
       <c r="Q11" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P11&gt;0.7,"A",IF(P11&gt;0.1,"B","C"))</f>
         <v>B</v>
       </c>
       <c r="R11" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F12:F1010,D12:D1010,M11)</f>
         <v>59</v>
       </c>
       <c r="S11" s="1">
-        <f t="shared" si="6"/>
+        <f>R11/O11</f>
         <v>2.2692307692307692</v>
       </c>
       <c r="T11" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S11-1)/4)</f>
         <v>0.68269230769230771</v>
       </c>
       <c r="U11" s="3">
-        <f t="shared" si="3"/>
+        <f>(P11+T11+Z11)/3</f>
         <v>0.32705128205128209</v>
       </c>
       <c r="V11" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D11:D1009,M11,E11:E1009,"1")/O11</f>
         <v>0</v>
       </c>
       <c r="W11" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D11:D1009,M11,E11:E1009,"2")/O11</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="X11" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D11:D1009,M11,E11:E1009,"3")/O11</f>
         <v>0.92307692307692313</v>
       </c>
       <c r="Y11" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E11:E1009,D11:D1009,M11)/O11</f>
         <v>2.9230769230769229</v>
       </c>
       <c r="Z11" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y11-1)/2)</f>
         <v>3.8461538461538547E-2</v>
       </c>
       <c r="AA11" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D11:D1009,M11,G11:G1009,"1")/O11</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="AB11" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D11:D1009,M11,G11:G1009,"2")/O11</f>
         <v>0.26923076923076922</v>
       </c>
       <c r="AC11" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D11:D1009,M11,G11:G1009,"3")/O11</f>
         <v>0.53846153846153844</v>
       </c>
       <c r="AD11" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D12:D1009,M11,H12:H1009,"1")+COUNTIFS(D12:D1009,M11,H12:H1009,"1,2"))/O11</f>
         <v>0.96153846153846156</v>
       </c>
       <c r="AE11" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D12:D1009,M11,H12:H1009,"2")+COUNTIFS(D12:D1009,M11,H12:H1009,"1,2"))/O11</f>
         <v>0.34615384615384615</v>
       </c>
       <c r="AF11" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D12:D1009,M11,I12:I1009,"1")+COUNTIFS(D12:D1009,M11,I12:I1009,"1,2")+COUNTIFS(D12:D1009,M11,I12:I1009,"1,3")+COUNTIFS(D12:D1009,M11,I12:I1009,"1,2,3"))/O11</f>
         <v>0.11538461538461539</v>
       </c>
       <c r="AG11" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D12:D1009,M11,I12:I1009,"2")+COUNTIFS(D12:D1009,M11,I12:I1009,"1,2")+COUNTIFS(D12:D1009,M11,I12:I1009,"2,3")+COUNTIFS(D12:D1009,M11,I12:I1009,"1,2,3"))/O11</f>
         <v>0.92307692307692313</v>
       </c>
       <c r="AH11" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D12:D1009,M11,I12:I1009,"3")+COUNTIFS(D12:D1009,M11,I12:I1009,"1,3")+COUNTIFS(D12:D1009,M11,I12:I1009,"2,3")+COUNTIFS(D12:D1009,M11,I12:I1009,"1,2,3"))/O11</f>
         <v>0.11538461538461539</v>
       </c>
       <c r="AI11" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D12:D1009,M11,J12:J1009,"1")+COUNTIFS(D12:D1009,M11,J12:J1009,"1,2")+COUNTIFS(D12:D1009,M11,J12:J1009,"1,3")+COUNTIFS(D12:D1009,M11,J12:J1009,"1,2,3"))/O11</f>
         <v>0.57692307692307687</v>
       </c>
       <c r="AJ11" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D12:D1009,M11,J12:J1009,"2")+COUNTIFS(D12:D1009,M11,J12:J1009,"1,2")+COUNTIFS(D12:D1009,M11,J12:J1009,"2,3")+COUNTIFS(D12:D1009,M11,J12:J1009,"1,2,3"))/O11</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="AK11" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D12:D1009,M11,J12:J1009,"3+X3")+COUNTIFS(D12:D1009,M11,J12:J1009,"1,3")+COUNTIFS(D12:D1009,M11,J12:J1009,"2,3")+COUNTIFS(D12:D1009,M11,J12:J1009,"1,2,3"))/O11</f>
         <v>0.23076923076923078</v>
       </c>
       <c r="AL11" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D11:D1009,M11,K11:K1009,"1")/O11</f>
         <v>0.38461538461538464</v>
       </c>
       <c r="AM11" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D11:D1009,M11,K11:K1009,"2")/O11</f>
         <v>0.30769230769230771</v>
       </c>
       <c r="AN11" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D11:D1009,M11,K11:K1009,"3")/O11</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="AO11" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D11:D1009,M11,K11:K1009,"4")/O11</f>
         <v>0.11538461538461539</v>
       </c>
     </row>
@@ -6501,111 +6463,111 @@
         <v>82</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D13:D1011,M12)</f>
         <v>17</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" si="27"/>
+        <f>O12/$M$32</f>
         <v>0.17</v>
       </c>
       <c r="Q12" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P12&gt;0.7,"A",IF(P12&gt;0.1,"B","C"))</f>
         <v>B</v>
       </c>
       <c r="R12" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F13:F1011,D13:D1011,M12)</f>
         <v>28</v>
       </c>
       <c r="S12" s="1">
-        <f t="shared" si="6"/>
+        <f>R12/O12</f>
         <v>1.6470588235294117</v>
       </c>
       <c r="T12" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S12-1)/4)</f>
         <v>0.83823529411764708</v>
       </c>
       <c r="U12" s="3">
-        <f t="shared" si="3"/>
+        <f>(P12+T12+Z12)/3</f>
         <v>0.52235294117647058</v>
       </c>
       <c r="V12" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D12:D1010,M12,E12:E1010,"1")/O12</f>
         <v>0.47058823529411764</v>
       </c>
       <c r="W12" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D12:D1010,M12,E12:E1010,"2")/O12</f>
         <v>0.17647058823529413</v>
       </c>
       <c r="X12" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D12:D1010,M12,E12:E1010,"3")/O12</f>
         <v>0.35294117647058826</v>
       </c>
       <c r="Y12" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E12:E1010,D12:D1010,M12)/O12</f>
         <v>1.8823529411764706</v>
       </c>
       <c r="Z12" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y12-1)/2)</f>
         <v>0.55882352941176472</v>
       </c>
       <c r="AA12" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D12:D1010,M12,G12:G1010,"1")/O12</f>
         <v>0</v>
       </c>
       <c r="AB12" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D12:D1010,M12,G12:G1010,"2")/O12</f>
         <v>0.17647058823529413</v>
       </c>
       <c r="AC12" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D12:D1010,M12,G12:G1010,"3")/O12</f>
         <v>0.82352941176470584</v>
       </c>
       <c r="AD12" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D13:D1010,M12,H13:H1010,"1")+COUNTIFS(D13:D1010,M12,H13:H1010,"1,2"))/O12</f>
         <v>1</v>
       </c>
       <c r="AE12" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D13:D1010,M12,H13:H1010,"2")+COUNTIFS(D13:D1010,M12,H13:H1010,"1,2"))/O12</f>
         <v>0.76470588235294112</v>
       </c>
       <c r="AF12" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D13:D1010,M12,I13:I1010,"1")+COUNTIFS(D13:D1010,M12,I13:I1010,"1,2")+COUNTIFS(D13:D1010,M12,I13:I1010,"1,3")+COUNTIFS(D13:D1010,M12,I13:I1010,"1,2,3"))/O12</f>
         <v>0.47058823529411764</v>
       </c>
       <c r="AG12" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D13:D1010,M12,I13:I1010,"2")+COUNTIFS(D13:D1010,M12,I13:I1010,"1,2")+COUNTIFS(D13:D1010,M12,I13:I1010,"2,3")+COUNTIFS(D13:D1010,M12,I13:I1010,"1,2,3"))/O12</f>
         <v>0.94117647058823528</v>
       </c>
       <c r="AH12" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D13:D1010,M12,I13:I1010,"3")+COUNTIFS(D13:D1010,M12,I13:I1010,"1,3")+COUNTIFS(D13:D1010,M12,I13:I1010,"2,3")+COUNTIFS(D13:D1010,M12,I13:I1010,"1,2,3"))/O12</f>
         <v>0.82352941176470584</v>
       </c>
       <c r="AI12" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D13:D1010,M12,J13:J1010,"1")+COUNTIFS(D13:D1010,M12,J13:J1010,"1,2")+COUNTIFS(D13:D1010,M12,J13:J1010,"1,3")+COUNTIFS(D13:D1010,M12,J13:J1010,"1,2,3"))/O12</f>
         <v>0.6470588235294118</v>
       </c>
       <c r="AJ12" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D13:D1010,M12,J13:J1010,"2")+COUNTIFS(D13:D1010,M12,J13:J1010,"1,2")+COUNTIFS(D13:D1010,M12,J13:J1010,"2,3")+COUNTIFS(D13:D1010,M12,J13:J1010,"1,2,3"))/O12</f>
         <v>0.29411764705882354</v>
       </c>
       <c r="AK12" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D13:D1010,M12,J13:J1010,"3+X3")+COUNTIFS(D13:D1010,M12,J13:J1010,"1,3")+COUNTIFS(D13:D1010,M12,J13:J1010,"2,3")+COUNTIFS(D13:D1010,M12,J13:J1010,"1,2,3"))/O12</f>
         <v>0.70588235294117652</v>
       </c>
       <c r="AL12" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D12:D1010,M12,K12:K1010,"1")/O12</f>
         <v>0.41176470588235292</v>
       </c>
       <c r="AM12" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D12:D1010,M12,K12:K1010,"2")/O12</f>
         <v>0.35294117647058826</v>
       </c>
       <c r="AN12" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D12:D1010,M12,K12:K1010,"3")/O12</f>
         <v>0</v>
       </c>
       <c r="AO12" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D12:D1010,M12,K12:K1010,"4")/O12</f>
         <v>0.23529411764705882</v>
       </c>
     </row>
@@ -6647,114 +6609,114 @@
         <v>25</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D14:D1012,M13)</f>
         <v>9</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" si="27"/>
+        <f>O13/$M$32</f>
         <v>0.09</v>
       </c>
       <c r="Q13" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P13&gt;0.7,"A",IF(P13&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R13" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F14:F1012,D14:D1012,M13)</f>
         <v>16</v>
       </c>
       <c r="S13" s="1">
-        <f t="shared" si="6"/>
+        <f>R13/O13</f>
         <v>1.7777777777777777</v>
       </c>
       <c r="T13" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S13-1)/4)</f>
         <v>0.80555555555555558</v>
       </c>
       <c r="U13" s="3">
-        <f t="shared" si="3"/>
+        <f>(P13+T13+Z13)/3</f>
         <v>0.5948148148148148</v>
       </c>
       <c r="V13" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D13:D1011,M13,E13:E1011,"1")/O13</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="W13" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D13:D1011,M13,E13:E1011,"2")/O13</f>
         <v>0</v>
       </c>
       <c r="X13" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D13:D1011,M13,E13:E1011,"3")/O13</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="Y13" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E13:E1011,D13:D1011,M13)/O13</f>
         <v>1.2222222222222223</v>
       </c>
       <c r="Z13" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y13-1)/2)</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="AA13" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D13:D1011,M13,G13:G1011,"1")/O13</f>
         <v>0</v>
       </c>
       <c r="AB13" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D13:D1011,M13,G13:G1011,"2")/O13</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="AC13" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D13:D1011,M13,G13:G1011,"3")/O13</f>
         <v>0.77777777777777779</v>
       </c>
       <c r="AD13" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D14:D1011,M13,H14:H1011,"1")+COUNTIFS(D14:D1011,M13,H14:H1011,"1,2"))/O13</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AE13" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D14:D1011,M13,H14:H1011,"2")+COUNTIFS(D14:D1011,M13,H14:H1011,"1,2"))/O13</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="AF13" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D14:D1011,M13,I14:I1011,"1")+COUNTIFS(D14:D1011,M13,I14:I1011,"1,2")+COUNTIFS(D14:D1011,M13,I14:I1011,"1,3")+COUNTIFS(D14:D1011,M13,I14:I1011,"1,2,3"))/O13</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AG13" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D14:D1011,M13,I14:I1011,"2")+COUNTIFS(D14:D1011,M13,I14:I1011,"1,2")+COUNTIFS(D14:D1011,M13,I14:I1011,"2,3")+COUNTIFS(D14:D1011,M13,I14:I1011,"1,2,3"))/O13</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="AH13" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D14:D1011,M13,I14:I1011,"3")+COUNTIFS(D14:D1011,M13,I14:I1011,"1,3")+COUNTIFS(D14:D1011,M13,I14:I1011,"2,3")+COUNTIFS(D14:D1011,M13,I14:I1011,"1,2,3"))/O13</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="AI13" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D14:D1011,M13,J14:J1011,"1")+COUNTIFS(D14:D1011,M13,J14:J1011,"1,2")+COUNTIFS(D14:D1011,M13,J14:J1011,"1,3")+COUNTIFS(D14:D1011,M13,J14:J1011,"1,2,3"))/O13</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AJ13" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D14:D1011,M13,J14:J1011,"2")+COUNTIFS(D14:D1011,M13,J14:J1011,"1,2")+COUNTIFS(D14:D1011,M13,J14:J1011,"2,3")+COUNTIFS(D14:D1011,M13,J14:J1011,"1,2,3"))/O13</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AK13" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D14:D1011,M13,J14:J1011,"3+X3")+COUNTIFS(D14:D1011,M13,J14:J1011,"1,3")+COUNTIFS(D14:D1011,M13,J14:J1011,"2,3")+COUNTIFS(D14:D1011,M13,J14:J1011,"1,2,3"))/O13</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="AL13" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D13:D1011,M13,K13:K1011,"1")/O13</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AM13" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D13:D1011,M13,K13:K1011,"2")/O13</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="AN13" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D13:D1011,M13,K13:K1011,"3")/O13</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="AO13" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D13:D1011,M13,K13:K1011,"4")/O13</f>
         <v>0</v>
       </c>
     </row>
@@ -6799,111 +6761,111 @@
         <v>82</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D15:D1013,M14)</f>
         <v>6</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="27"/>
+        <f>O14/$M$32</f>
         <v>0.06</v>
       </c>
       <c r="Q14" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P14&gt;0.7,"A",IF(P14&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R14" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F15:F1013,D15:D1013,M14)</f>
         <v>14</v>
       </c>
       <c r="S14" s="1">
-        <f t="shared" si="6"/>
+        <f>R14/O14</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="T14" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S14-1)/4)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="U14" s="3">
-        <f t="shared" si="3"/>
+        <f>(P14+T14+Z14)/3</f>
         <v>0.46444444444444438</v>
       </c>
       <c r="V14" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D14:D1012,M14,E14:E1012,"1")/O14</f>
         <v>0.5</v>
       </c>
       <c r="W14" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D14:D1012,M14,E14:E1012,"2")/O14</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="X14" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D14:D1012,M14,E14:E1012,"3")/O14</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="Y14" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E14:E1012,D14:D1012,M14)/O14</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="Z14" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y14-1)/2)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AA14" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D14:D1012,M14,G14:G1012,"1")/O14</f>
         <v>0</v>
       </c>
       <c r="AB14" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D14:D1012,M14,G14:G1012,"2")/O14</f>
         <v>0</v>
       </c>
       <c r="AC14" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D14:D1012,M14,G14:G1012,"3")/O14</f>
         <v>1</v>
       </c>
       <c r="AD14" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D15:D1012,M14,H15:H1012,"1")+COUNTIFS(D15:D1012,M14,H15:H1012,"1,2"))/O14</f>
         <v>1</v>
       </c>
       <c r="AE14" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D15:D1012,M14,H15:H1012,"2")+COUNTIFS(D15:D1012,M14,H15:H1012,"1,2"))/O14</f>
         <v>0.5</v>
       </c>
       <c r="AF14" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D15:D1012,M14,I15:I1012,"1")+COUNTIFS(D15:D1012,M14,I15:I1012,"1,2")+COUNTIFS(D15:D1012,M14,I15:I1012,"1,3")+COUNTIFS(D15:D1012,M14,I15:I1012,"1,2,3"))/O14</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="AG14" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D15:D1012,M14,I15:I1012,"2")+COUNTIFS(D15:D1012,M14,I15:I1012,"1,2")+COUNTIFS(D15:D1012,M14,I15:I1012,"2,3")+COUNTIFS(D15:D1012,M14,I15:I1012,"1,2,3"))/O14</f>
         <v>0.5</v>
       </c>
       <c r="AH14" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D15:D1012,M14,I15:I1012,"3")+COUNTIFS(D15:D1012,M14,I15:I1012,"1,3")+COUNTIFS(D15:D1012,M14,I15:I1012,"2,3")+COUNTIFS(D15:D1012,M14,I15:I1012,"1,2,3"))/O14</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AI14" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D15:D1012,M14,J15:J1012,"1")+COUNTIFS(D15:D1012,M14,J15:J1012,"1,2")+COUNTIFS(D15:D1012,M14,J15:J1012,"1,3")+COUNTIFS(D15:D1012,M14,J15:J1012,"1,2,3"))/O14</f>
         <v>0.5</v>
       </c>
       <c r="AJ14" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D15:D1012,M14,J15:J1012,"2")+COUNTIFS(D15:D1012,M14,J15:J1012,"1,2")+COUNTIFS(D15:D1012,M14,J15:J1012,"2,3")+COUNTIFS(D15:D1012,M14,J15:J1012,"1,2,3"))/O14</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="AK14" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D15:D1012,M14,J15:J1012,"3+X3")+COUNTIFS(D15:D1012,M14,J15:J1012,"1,3")+COUNTIFS(D15:D1012,M14,J15:J1012,"2,3")+COUNTIFS(D15:D1012,M14,J15:J1012,"1,2,3"))/O14</f>
         <v>0.5</v>
       </c>
       <c r="AL14" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D14:D1012,M14,K14:K1012,"1")/O14</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AM14" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D14:D1012,M14,K14:K1012,"2")/O14</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="AN14" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D14:D1012,M14,K14:K1012,"3")/O14</f>
         <v>0</v>
       </c>
       <c r="AO14" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D14:D1012,M14,K14:K1012,"4")/O14</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -6945,114 +6907,114 @@
         <v>29</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D16:D1014,M15)</f>
         <v>5</v>
       </c>
       <c r="P15" s="3">
-        <f t="shared" si="27"/>
+        <f>O15/$M$32</f>
         <v>0.05</v>
       </c>
       <c r="Q15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P15&gt;0.7,"A",IF(P15&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R15" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F16:F1014,D16:D1014,M15)</f>
         <v>10</v>
       </c>
       <c r="S15" s="1">
-        <f t="shared" si="6"/>
+        <f>R15/O15</f>
         <v>2</v>
       </c>
       <c r="T15" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S15-1)/4)</f>
         <v>0.75</v>
       </c>
       <c r="U15" s="3">
-        <f t="shared" si="3"/>
+        <f>(P15+T15+Z15)/3</f>
         <v>0.43333333333333335</v>
       </c>
       <c r="V15" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D15:D1013,M15,E15:E1013,"1")/O15</f>
         <v>0.2</v>
       </c>
       <c r="W15" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D15:D1013,M15,E15:E1013,"2")/O15</f>
         <v>0.6</v>
       </c>
       <c r="X15" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D15:D1013,M15,E15:E1013,"3")/O15</f>
         <v>0.2</v>
       </c>
       <c r="Y15" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E15:E1013,D15:D1013,M15)/O15</f>
         <v>2</v>
       </c>
       <c r="Z15" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y15-1)/2)</f>
         <v>0.5</v>
       </c>
       <c r="AA15" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D15:D1013,M15,G15:G1013,"1")/O15</f>
         <v>0</v>
       </c>
       <c r="AB15" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D15:D1013,M15,G15:G1013,"2")/O15</f>
         <v>0.4</v>
       </c>
       <c r="AC15" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D15:D1013,M15,G15:G1013,"3")/O15</f>
         <v>0.4</v>
       </c>
       <c r="AD15" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D16:D1013,M15,H16:H1013,"1")+COUNTIFS(D16:D1013,M15,H16:H1013,"1,2"))/O15</f>
         <v>1</v>
       </c>
       <c r="AE15" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D16:D1013,M15,H16:H1013,"2")+COUNTIFS(D16:D1013,M15,H16:H1013,"1,2"))/O15</f>
         <v>0</v>
       </c>
       <c r="AF15" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D16:D1013,M15,I16:I1013,"1")+COUNTIFS(D16:D1013,M15,I16:I1013,"1,2")+COUNTIFS(D16:D1013,M15,I16:I1013,"1,3")+COUNTIFS(D16:D1013,M15,I16:I1013,"1,2,3"))/O15</f>
         <v>0.6</v>
       </c>
       <c r="AG15" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D16:D1013,M15,I16:I1013,"2")+COUNTIFS(D16:D1013,M15,I16:I1013,"1,2")+COUNTIFS(D16:D1013,M15,I16:I1013,"2,3")+COUNTIFS(D16:D1013,M15,I16:I1013,"1,2,3"))/O15</f>
         <v>0.4</v>
       </c>
       <c r="AH15" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D16:D1013,M15,I16:I1013,"3")+COUNTIFS(D16:D1013,M15,I16:I1013,"1,3")+COUNTIFS(D16:D1013,M15,I16:I1013,"2,3")+COUNTIFS(D16:D1013,M15,I16:I1013,"1,2,3"))/O15</f>
         <v>0</v>
       </c>
       <c r="AI15" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D16:D1013,M15,J16:J1013,"1")+COUNTIFS(D16:D1013,M15,J16:J1013,"1,2")+COUNTIFS(D16:D1013,M15,J16:J1013,"1,3")+COUNTIFS(D16:D1013,M15,J16:J1013,"1,2,3"))/O15</f>
         <v>0.8</v>
       </c>
       <c r="AJ15" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D16:D1013,M15,J16:J1013,"2")+COUNTIFS(D16:D1013,M15,J16:J1013,"1,2")+COUNTIFS(D16:D1013,M15,J16:J1013,"2,3")+COUNTIFS(D16:D1013,M15,J16:J1013,"1,2,3"))/O15</f>
         <v>0</v>
       </c>
       <c r="AK15" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D16:D1013,M15,J16:J1013,"3+X3")+COUNTIFS(D16:D1013,M15,J16:J1013,"1,3")+COUNTIFS(D16:D1013,M15,J16:J1013,"2,3")+COUNTIFS(D16:D1013,M15,J16:J1013,"1,2,3"))/O15</f>
         <v>0.2</v>
       </c>
       <c r="AL15" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D15:D1013,M15,K15:K1013,"1")/O15</f>
         <v>0.8</v>
       </c>
       <c r="AM15" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D15:D1013,M15,K15:K1013,"2")/O15</f>
         <v>0</v>
       </c>
       <c r="AN15" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D15:D1013,M15,K15:K1013,"3")/O15</f>
         <v>0</v>
       </c>
       <c r="AO15" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D15:D1013,M15,K15:K1013,"4")/O15</f>
         <v>0.2</v>
       </c>
     </row>
@@ -7094,114 +7056,114 @@
         <v>23</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D17:D1015,M16)</f>
         <v>4</v>
       </c>
       <c r="P16" s="3">
-        <f t="shared" si="27"/>
+        <f>O16/$M$32</f>
         <v>0.04</v>
       </c>
       <c r="Q16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P16&gt;0.7,"A",IF(P16&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R16" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F17:F1015,D17:D1015,M16)</f>
         <v>11</v>
       </c>
       <c r="S16" s="1">
-        <f t="shared" si="6"/>
+        <f>R16/O16</f>
         <v>2.75</v>
       </c>
       <c r="T16" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S16-1)/4)</f>
         <v>0.5625</v>
       </c>
       <c r="U16" s="3">
-        <f t="shared" si="3"/>
+        <f>(P16+T16+Z16)/3</f>
         <v>0.45083333333333336</v>
       </c>
       <c r="V16" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D16:D1014,M16,E16:E1014,"1")/O16</f>
         <v>0.75</v>
       </c>
       <c r="W16" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D16:D1014,M16,E16:E1014,"2")/O16</f>
         <v>0</v>
       </c>
       <c r="X16" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D16:D1014,M16,E16:E1014,"3")/O16</f>
         <v>0.25</v>
       </c>
       <c r="Y16" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E16:E1014,D16:D1014,M16)/O16</f>
         <v>1.5</v>
       </c>
       <c r="Z16" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y16-1)/2)</f>
         <v>0.75</v>
       </c>
       <c r="AA16" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D16:D1014,M16,G16:G1014,"1")/O16</f>
         <v>0</v>
       </c>
       <c r="AB16" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D16:D1014,M16,G16:G1014,"2")/O16</f>
         <v>0.25</v>
       </c>
       <c r="AC16" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D16:D1014,M16,G16:G1014,"3")/O16</f>
         <v>0.75</v>
       </c>
       <c r="AD16" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D17:D1014,M16,H17:H1014,"1")+COUNTIFS(D17:D1014,M16,H17:H1014,"1,2"))/O16</f>
         <v>1</v>
       </c>
       <c r="AE16" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D17:D1014,M16,H17:H1014,"2")+COUNTIFS(D17:D1014,M16,H17:H1014,"1,2"))/O16</f>
         <v>0.5</v>
       </c>
       <c r="AF16" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D17:D1014,M16,I17:I1014,"1")+COUNTIFS(D17:D1014,M16,I17:I1014,"1,2")+COUNTIFS(D17:D1014,M16,I17:I1014,"1,3")+COUNTIFS(D17:D1014,M16,I17:I1014,"1,2,3"))/O16</f>
         <v>0.75</v>
       </c>
       <c r="AG16" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D17:D1014,M16,I17:I1014,"2")+COUNTIFS(D17:D1014,M16,I17:I1014,"1,2")+COUNTIFS(D17:D1014,M16,I17:I1014,"2,3")+COUNTIFS(D17:D1014,M16,I17:I1014,"1,2,3"))/O16</f>
         <v>0.75</v>
       </c>
       <c r="AH16" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D17:D1014,M16,I17:I1014,"3")+COUNTIFS(D17:D1014,M16,I17:I1014,"1,3")+COUNTIFS(D17:D1014,M16,I17:I1014,"2,3")+COUNTIFS(D17:D1014,M16,I17:I1014,"1,2,3"))/O16</f>
         <v>0.5</v>
       </c>
       <c r="AI16" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D17:D1014,M16,J17:J1014,"1")+COUNTIFS(D17:D1014,M16,J17:J1014,"1,2")+COUNTIFS(D17:D1014,M16,J17:J1014,"1,3")+COUNTIFS(D17:D1014,M16,J17:J1014,"1,2,3"))/O16</f>
         <v>0.75</v>
       </c>
       <c r="AJ16" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D17:D1014,M16,J17:J1014,"2")+COUNTIFS(D17:D1014,M16,J17:J1014,"1,2")+COUNTIFS(D17:D1014,M16,J17:J1014,"2,3")+COUNTIFS(D17:D1014,M16,J17:J1014,"1,2,3"))/O16</f>
         <v>0.5</v>
       </c>
       <c r="AK16" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D17:D1014,M16,J17:J1014,"3+X3")+COUNTIFS(D17:D1014,M16,J17:J1014,"1,3")+COUNTIFS(D17:D1014,M16,J17:J1014,"2,3")+COUNTIFS(D17:D1014,M16,J17:J1014,"1,2,3"))/O16</f>
         <v>0.5</v>
       </c>
       <c r="AL16" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D16:D1014,M16,K16:K1014,"1")/O16</f>
         <v>0.5</v>
       </c>
       <c r="AM16" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D16:D1014,M16,K16:K1014,"2")/O16</f>
         <v>0.25</v>
       </c>
       <c r="AN16" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D16:D1014,M16,K16:K1014,"3")/O16</f>
         <v>0</v>
       </c>
       <c r="AO16" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D16:D1014,M16,K16:K1014,"4")/O16</f>
         <v>0.25</v>
       </c>
     </row>
@@ -7246,111 +7208,111 @@
         <v>83</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D18:D1016,M17)</f>
         <v>4</v>
       </c>
       <c r="P17" s="3">
-        <f t="shared" si="27"/>
+        <f>O17/$M$32</f>
         <v>0.04</v>
       </c>
       <c r="Q17" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P17&gt;0.7,"A",IF(P17&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F18:F1016,D18:D1016,M17)</f>
         <v>6</v>
       </c>
       <c r="S17" s="1">
-        <f t="shared" si="6"/>
+        <f>R17/O17</f>
         <v>1.5</v>
       </c>
       <c r="T17" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S17-1)/4)</f>
         <v>0.875</v>
       </c>
       <c r="U17" s="3">
-        <f t="shared" si="3"/>
+        <f>(P17+T17+Z17)/3</f>
         <v>0.34666666666666668</v>
       </c>
       <c r="V17" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D17:D1015,M17,E17:E1015,"1")/O17</f>
         <v>0</v>
       </c>
       <c r="W17" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D17:D1015,M17,E17:E1015,"2")/O17</f>
         <v>0.25</v>
       </c>
       <c r="X17" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D17:D1015,M17,E17:E1015,"3")/O17</f>
         <v>0.75</v>
       </c>
       <c r="Y17" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E17:E1015,D17:D1015,M17)/O17</f>
         <v>2.75</v>
       </c>
       <c r="Z17" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y17-1)/2)</f>
         <v>0.125</v>
       </c>
       <c r="AA17" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D17:D1015,M17,G17:G1015,"1")/O17</f>
         <v>0</v>
       </c>
       <c r="AB17" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D17:D1015,M17,G17:G1015,"2")/O17</f>
         <v>0.75</v>
       </c>
       <c r="AC17" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D17:D1015,M17,G17:G1015,"3")/O17</f>
         <v>0.25</v>
       </c>
       <c r="AD17" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D18:D1015,M17,H18:H1015,"1")+COUNTIFS(D18:D1015,M17,H18:H1015,"1,2"))/O17</f>
         <v>1</v>
       </c>
       <c r="AE17" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D18:D1015,M17,H18:H1015,"2")+COUNTIFS(D18:D1015,M17,H18:H1015,"1,2"))/O17</f>
         <v>0.5</v>
       </c>
       <c r="AF17" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D18:D1015,M17,I18:I1015,"1")+COUNTIFS(D18:D1015,M17,I18:I1015,"1,2")+COUNTIFS(D18:D1015,M17,I18:I1015,"1,3")+COUNTIFS(D18:D1015,M17,I18:I1015,"1,2,3"))/O17</f>
         <v>0</v>
       </c>
       <c r="AG17" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D18:D1015,M17,I18:I1015,"2")+COUNTIFS(D18:D1015,M17,I18:I1015,"1,2")+COUNTIFS(D18:D1015,M17,I18:I1015,"2,3")+COUNTIFS(D18:D1015,M17,I18:I1015,"1,2,3"))/O17</f>
         <v>1</v>
       </c>
       <c r="AH17" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D18:D1015,M17,I18:I1015,"3")+COUNTIFS(D18:D1015,M17,I18:I1015,"1,3")+COUNTIFS(D18:D1015,M17,I18:I1015,"2,3")+COUNTIFS(D18:D1015,M17,I18:I1015,"1,2,3"))/O17</f>
         <v>0.25</v>
       </c>
       <c r="AI17" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D18:D1015,M17,J18:J1015,"1")+COUNTIFS(D18:D1015,M17,J18:J1015,"1,2")+COUNTIFS(D18:D1015,M17,J18:J1015,"1,3")+COUNTIFS(D18:D1015,M17,J18:J1015,"1,2,3"))/O17</f>
         <v>1</v>
       </c>
       <c r="AJ17" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D18:D1015,M17,J18:J1015,"2")+COUNTIFS(D18:D1015,M17,J18:J1015,"1,2")+COUNTIFS(D18:D1015,M17,J18:J1015,"2,3")+COUNTIFS(D18:D1015,M17,J18:J1015,"1,2,3"))/O17</f>
         <v>0</v>
       </c>
       <c r="AK17" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D18:D1015,M17,J18:J1015,"3+X3")+COUNTIFS(D18:D1015,M17,J18:J1015,"1,3")+COUNTIFS(D18:D1015,M17,J18:J1015,"2,3")+COUNTIFS(D18:D1015,M17,J18:J1015,"1,2,3"))/O17</f>
         <v>0</v>
       </c>
       <c r="AL17" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D17:D1015,M17,K17:K1015,"1")/O17</f>
         <v>0.25</v>
       </c>
       <c r="AM17" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D17:D1015,M17,K17:K1015,"2")/O17</f>
         <v>0.75</v>
       </c>
       <c r="AN17" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D17:D1015,M17,K17:K1015,"3")/O17</f>
         <v>0</v>
       </c>
       <c r="AO17" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D17:D1015,M17,K17:K1015,"4")/O17</f>
         <v>0</v>
       </c>
     </row>
@@ -7395,111 +7357,111 @@
         <v>82</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D19:D1017,M18)</f>
         <v>3</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" si="27"/>
+        <f>O18/$M$32</f>
         <v>0.03</v>
       </c>
       <c r="Q18" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P18&gt;0.7,"A",IF(P18&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R18" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F19:F1017,D19:D1017,M18)</f>
         <v>5</v>
       </c>
       <c r="S18" s="1">
-        <f t="shared" si="6"/>
+        <f>R18/O18</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="T18" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S18-1)/4)</f>
         <v>0.83333333333333326</v>
       </c>
       <c r="U18" s="3">
-        <f t="shared" si="3"/>
+        <f>(P18+T18+Z18)/3</f>
         <v>0.62111111111111106</v>
       </c>
       <c r="V18" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D18:D1016,M18,E18:E1016,"1")/O18</f>
         <v>1</v>
       </c>
       <c r="W18" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D18:D1016,M18,E18:E1016,"2")/O18</f>
         <v>0</v>
       </c>
       <c r="X18" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D18:D1016,M18,E18:E1016,"3")/O18</f>
         <v>0</v>
       </c>
       <c r="Y18" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E18:E1016,D18:D1016,M18)/O18</f>
         <v>1</v>
       </c>
       <c r="Z18" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y18-1)/2)</f>
         <v>1</v>
       </c>
       <c r="AA18" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D18:D1016,M18,G18:G1016,"1")/O18</f>
         <v>0</v>
       </c>
       <c r="AB18" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D18:D1016,M18,G18:G1016,"2")/O18</f>
         <v>0</v>
       </c>
       <c r="AC18" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D18:D1016,M18,G18:G1016,"3")/O18</f>
         <v>1</v>
       </c>
       <c r="AD18" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D19:D1016,M18,H19:H1016,"1")+COUNTIFS(D19:D1016,M18,H19:H1016,"1,2"))/O18</f>
         <v>1</v>
       </c>
       <c r="AE18" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D19:D1016,M18,H19:H1016,"2")+COUNTIFS(D19:D1016,M18,H19:H1016,"1,2"))/O18</f>
         <v>1</v>
       </c>
       <c r="AF18" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D19:D1016,M18,I19:I1016,"1")+COUNTIFS(D19:D1016,M18,I19:I1016,"1,2")+COUNTIFS(D19:D1016,M18,I19:I1016,"1,3")+COUNTIFS(D19:D1016,M18,I19:I1016,"1,2,3"))/O18</f>
         <v>1</v>
       </c>
       <c r="AG18" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D19:D1016,M18,I19:I1016,"2")+COUNTIFS(D19:D1016,M18,I19:I1016,"1,2")+COUNTIFS(D19:D1016,M18,I19:I1016,"2,3")+COUNTIFS(D19:D1016,M18,I19:I1016,"1,2,3"))/O18</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AH18" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D19:D1016,M18,I19:I1016,"3")+COUNTIFS(D19:D1016,M18,I19:I1016,"1,3")+COUNTIFS(D19:D1016,M18,I19:I1016,"2,3")+COUNTIFS(D19:D1016,M18,I19:I1016,"1,2,3"))/O18</f>
         <v>1</v>
       </c>
       <c r="AI18" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D19:D1016,M18,J19:J1016,"1")+COUNTIFS(D19:D1016,M18,J19:J1016,"1,2")+COUNTIFS(D19:D1016,M18,J19:J1016,"1,3")+COUNTIFS(D19:D1016,M18,J19:J1016,"1,2,3"))/O18</f>
         <v>1</v>
       </c>
       <c r="AJ18" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D19:D1016,M18,J19:J1016,"2")+COUNTIFS(D19:D1016,M18,J19:J1016,"1,2")+COUNTIFS(D19:D1016,M18,J19:J1016,"2,3")+COUNTIFS(D19:D1016,M18,J19:J1016,"1,2,3"))/O18</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AK18" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D19:D1016,M18,J19:J1016,"3+X3")+COUNTIFS(D19:D1016,M18,J19:J1016,"1,3")+COUNTIFS(D19:D1016,M18,J19:J1016,"2,3")+COUNTIFS(D19:D1016,M18,J19:J1016,"1,2,3"))/O18</f>
         <v>1</v>
       </c>
       <c r="AL18" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D18:D1016,M18,K18:K1016,"1")/O18</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AM18" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D18:D1016,M18,K18:K1016,"2")/O18</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AN18" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D18:D1016,M18,K18:K1016,"3")/O18</f>
         <v>0</v>
       </c>
       <c r="AO18" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D18:D1016,M18,K18:K1016,"4")/O18</f>
         <v>0</v>
       </c>
     </row>
@@ -7541,114 +7503,114 @@
         <v>28</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D20:D1018,M19)</f>
         <v>3</v>
       </c>
       <c r="P19" s="3">
-        <f t="shared" si="27"/>
+        <f>O19/$M$32</f>
         <v>0.03</v>
       </c>
       <c r="Q19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P19&gt;0.7,"A",IF(P19&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R19" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F20:F1018,D20:D1018,M19)</f>
         <v>7</v>
       </c>
       <c r="S19" s="1">
-        <f t="shared" si="6"/>
+        <f>R19/O19</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="T19" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S19-1)/4)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="U19" s="3">
-        <f t="shared" si="3"/>
+        <f>(P19+T19+Z19)/3</f>
         <v>0.51</v>
       </c>
       <c r="V19" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D19:D1017,M19,E19:E1017,"1")/O19</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="W19" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D19:D1017,M19,E19:E1017,"2")/O19</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="X19" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D19:D1017,M19,E19:E1017,"3")/O19</f>
         <v>0</v>
       </c>
       <c r="Y19" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E19:E1017,D19:D1017,M19)/O19</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="Z19" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y19-1)/2)</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="AA19" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D19:D1017,M19,G19:G1017,"1")/O19</f>
         <v>0</v>
       </c>
       <c r="AB19" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D19:D1017,M19,G19:G1017,"2")/O19</f>
         <v>0</v>
       </c>
       <c r="AC19" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D19:D1017,M19,G19:G1017,"3")/O19</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AD19" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D20:D1017,M19,H20:H1017,"1")+COUNTIFS(D20:D1017,M19,H20:H1017,"1,2"))/O19</f>
         <v>1</v>
       </c>
       <c r="AE19" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D20:D1017,M19,H20:H1017,"2")+COUNTIFS(D20:D1017,M19,H20:H1017,"1,2"))/O19</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AF19" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D20:D1017,M19,I20:I1017,"1")+COUNTIFS(D20:D1017,M19,I20:I1017,"1,2")+COUNTIFS(D20:D1017,M19,I20:I1017,"1,3")+COUNTIFS(D20:D1017,M19,I20:I1017,"1,2,3"))/O19</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AG19" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D20:D1017,M19,I20:I1017,"2")+COUNTIFS(D20:D1017,M19,I20:I1017,"1,2")+COUNTIFS(D20:D1017,M19,I20:I1017,"2,3")+COUNTIFS(D20:D1017,M19,I20:I1017,"1,2,3"))/O19</f>
         <v>1</v>
       </c>
       <c r="AH19" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D20:D1017,M19,I20:I1017,"3")+COUNTIFS(D20:D1017,M19,I20:I1017,"1,3")+COUNTIFS(D20:D1017,M19,I20:I1017,"2,3")+COUNTIFS(D20:D1017,M19,I20:I1017,"1,2,3"))/O19</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AI19" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D20:D1017,M19,J20:J1017,"1")+COUNTIFS(D20:D1017,M19,J20:J1017,"1,2")+COUNTIFS(D20:D1017,M19,J20:J1017,"1,3")+COUNTIFS(D20:D1017,M19,J20:J1017,"1,2,3"))/O19</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AJ19" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D20:D1017,M19,J20:J1017,"2")+COUNTIFS(D20:D1017,M19,J20:J1017,"1,2")+COUNTIFS(D20:D1017,M19,J20:J1017,"2,3")+COUNTIFS(D20:D1017,M19,J20:J1017,"1,2,3"))/O19</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AK19" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D20:D1017,M19,J20:J1017,"3+X3")+COUNTIFS(D20:D1017,M19,J20:J1017,"1,3")+COUNTIFS(D20:D1017,M19,J20:J1017,"2,3")+COUNTIFS(D20:D1017,M19,J20:J1017,"1,2,3"))/O19</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AL19" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D19:D1017,M19,K19:K1017,"1")/O19</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AM19" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D19:D1017,M19,K19:K1017,"2")/O19</f>
         <v>0</v>
       </c>
       <c r="AN19" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D19:D1017,M19,K19:K1017,"3")/O19</f>
         <v>0</v>
       </c>
       <c r="AO19" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D19:D1017,M19,K19:K1017,"4")/O19</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -7690,114 +7652,114 @@
         <v>20</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D21:D1019,M20)</f>
         <v>2</v>
       </c>
       <c r="P20" s="3">
-        <f t="shared" si="27"/>
+        <f>O20/$M$32</f>
         <v>0.02</v>
       </c>
       <c r="Q20" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P20&gt;0.7,"A",IF(P20&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R20" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F21:F1019,D21:D1019,M20)</f>
         <v>4</v>
       </c>
       <c r="S20" s="1">
-        <f t="shared" si="6"/>
+        <f>R20/O20</f>
         <v>2</v>
       </c>
       <c r="T20" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S20-1)/4)</f>
         <v>0.75</v>
       </c>
       <c r="U20" s="3">
-        <f t="shared" si="3"/>
+        <f>(P20+T20+Z20)/3</f>
         <v>0.34</v>
       </c>
       <c r="V20" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D20:D1018,M20,E20:E1018,"1")/O20</f>
         <v>0</v>
       </c>
       <c r="W20" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D20:D1018,M20,E20:E1018,"2")/O20</f>
         <v>0.5</v>
       </c>
       <c r="X20" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D20:D1018,M20,E20:E1018,"3")/O20</f>
         <v>0.5</v>
       </c>
       <c r="Y20" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E20:E1018,D20:D1018,M20)/O20</f>
         <v>2.5</v>
       </c>
       <c r="Z20" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y20-1)/2)</f>
         <v>0.25</v>
       </c>
       <c r="AA20" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D20:D1018,M20,G20:G1018,"1")/O20</f>
         <v>0</v>
       </c>
       <c r="AB20" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D20:D1018,M20,G20:G1018,"2")/O20</f>
         <v>0.5</v>
       </c>
       <c r="AC20" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D20:D1018,M20,G20:G1018,"3")/O20</f>
         <v>0</v>
       </c>
       <c r="AD20" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D21:D1018,M20,H21:H1018,"1")+COUNTIFS(D21:D1018,M20,H21:H1018,"1,2"))/O20</f>
         <v>1</v>
       </c>
       <c r="AE20" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D21:D1018,M20,H21:H1018,"2")+COUNTIFS(D21:D1018,M20,H21:H1018,"1,2"))/O20</f>
         <v>1</v>
       </c>
       <c r="AF20" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D21:D1018,M20,I21:I1018,"1")+COUNTIFS(D21:D1018,M20,I21:I1018,"1,2")+COUNTIFS(D21:D1018,M20,I21:I1018,"1,3")+COUNTIFS(D21:D1018,M20,I21:I1018,"1,2,3"))/O20</f>
         <v>0</v>
       </c>
       <c r="AG20" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D21:D1018,M20,I21:I1018,"2")+COUNTIFS(D21:D1018,M20,I21:I1018,"1,2")+COUNTIFS(D21:D1018,M20,I21:I1018,"2,3")+COUNTIFS(D21:D1018,M20,I21:I1018,"1,2,3"))/O20</f>
         <v>1</v>
       </c>
       <c r="AH20" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D21:D1018,M20,I21:I1018,"3")+COUNTIFS(D21:D1018,M20,I21:I1018,"1,3")+COUNTIFS(D21:D1018,M20,I21:I1018,"2,3")+COUNTIFS(D21:D1018,M20,I21:I1018,"1,2,3"))/O20</f>
         <v>1</v>
       </c>
       <c r="AI20" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D21:D1018,M20,J21:J1018,"1")+COUNTIFS(D21:D1018,M20,J21:J1018,"1,2")+COUNTIFS(D21:D1018,M20,J21:J1018,"1,3")+COUNTIFS(D21:D1018,M20,J21:J1018,"1,2,3"))/O20</f>
         <v>0.5</v>
       </c>
       <c r="AJ20" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D21:D1018,M20,J21:J1018,"2")+COUNTIFS(D21:D1018,M20,J21:J1018,"1,2")+COUNTIFS(D21:D1018,M20,J21:J1018,"2,3")+COUNTIFS(D21:D1018,M20,J21:J1018,"1,2,3"))/O20</f>
         <v>0</v>
       </c>
       <c r="AK20" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D21:D1018,M20,J21:J1018,"3+X3")+COUNTIFS(D21:D1018,M20,J21:J1018,"1,3")+COUNTIFS(D21:D1018,M20,J21:J1018,"2,3")+COUNTIFS(D21:D1018,M20,J21:J1018,"1,2,3"))/O20</f>
         <v>0.5</v>
       </c>
       <c r="AL20" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D20:D1018,M20,K20:K1018,"1")/O20</f>
         <v>0.5</v>
       </c>
       <c r="AM20" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D20:D1018,M20,K20:K1018,"2")/O20</f>
         <v>0.5</v>
       </c>
       <c r="AN20" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D20:D1018,M20,K20:K1018,"3")/O20</f>
         <v>0</v>
       </c>
       <c r="AO20" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D20:D1018,M20,K20:K1018,"4")/O20</f>
         <v>0</v>
       </c>
     </row>
@@ -7839,114 +7801,114 @@
         <v>26</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D22:D1020,M21)</f>
         <v>2</v>
       </c>
       <c r="P21" s="3">
-        <f t="shared" si="27"/>
+        <f>O21/$M$32</f>
         <v>0.02</v>
       </c>
       <c r="Q21" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P21&gt;0.7,"A",IF(P21&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R21" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F22:F1020,D22:D1020,M21)</f>
         <v>2</v>
       </c>
       <c r="S21" s="1">
-        <f t="shared" si="6"/>
+        <f>R21/O21</f>
         <v>1</v>
       </c>
       <c r="T21" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S21-1)/4)</f>
         <v>1</v>
       </c>
       <c r="U21" s="3">
-        <f t="shared" si="3"/>
+        <f>(P21+T21+Z21)/3</f>
         <v>0.67333333333333334</v>
       </c>
       <c r="V21" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D21:D1019,M21,E21:E1019,"1")/O21</f>
         <v>1</v>
       </c>
       <c r="W21" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D21:D1019,M21,E21:E1019,"2")/O21</f>
         <v>0</v>
       </c>
       <c r="X21" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D21:D1019,M21,E21:E1019,"3")/O21</f>
         <v>0</v>
       </c>
       <c r="Y21" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E21:E1019,D21:D1019,M21)/O21</f>
         <v>1</v>
       </c>
       <c r="Z21" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y21-1)/2)</f>
         <v>1</v>
       </c>
       <c r="AA21" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D21:D1019,M21,G21:G1019,"1")/O21</f>
         <v>0</v>
       </c>
       <c r="AB21" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D21:D1019,M21,G21:G1019,"2")/O21</f>
         <v>0</v>
       </c>
       <c r="AC21" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D21:D1019,M21,G21:G1019,"3")/O21</f>
         <v>1</v>
       </c>
       <c r="AD21" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D22:D1019,M21,H22:H1019,"1")+COUNTIFS(D22:D1019,M21,H22:H1019,"1,2"))/O21</f>
         <v>0</v>
       </c>
       <c r="AE21" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D22:D1019,M21,H22:H1019,"2")+COUNTIFS(D22:D1019,M21,H22:H1019,"1,2"))/O21</f>
         <v>1</v>
       </c>
       <c r="AF21" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D22:D1019,M21,I22:I1019,"1")+COUNTIFS(D22:D1019,M21,I22:I1019,"1,2")+COUNTIFS(D22:D1019,M21,I22:I1019,"1,3")+COUNTIFS(D22:D1019,M21,I22:I1019,"1,2,3"))/O21</f>
         <v>0.5</v>
       </c>
       <c r="AG21" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D22:D1019,M21,I22:I1019,"2")+COUNTIFS(D22:D1019,M21,I22:I1019,"1,2")+COUNTIFS(D22:D1019,M21,I22:I1019,"2,3")+COUNTIFS(D22:D1019,M21,I22:I1019,"1,2,3"))/O21</f>
         <v>0</v>
       </c>
       <c r="AH21" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D22:D1019,M21,I22:I1019,"3")+COUNTIFS(D22:D1019,M21,I22:I1019,"1,3")+COUNTIFS(D22:D1019,M21,I22:I1019,"2,3")+COUNTIFS(D22:D1019,M21,I22:I1019,"1,2,3"))/O21</f>
         <v>0.5</v>
       </c>
       <c r="AI21" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D22:D1019,M21,J22:J1019,"1")+COUNTIFS(D22:D1019,M21,J22:J1019,"1,2")+COUNTIFS(D22:D1019,M21,J22:J1019,"1,3")+COUNTIFS(D22:D1019,M21,J22:J1019,"1,2,3"))/O21</f>
         <v>0.5</v>
       </c>
       <c r="AJ21" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D22:D1019,M21,J22:J1019,"2")+COUNTIFS(D22:D1019,M21,J22:J1019,"1,2")+COUNTIFS(D22:D1019,M21,J22:J1019,"2,3")+COUNTIFS(D22:D1019,M21,J22:J1019,"1,2,3"))/O21</f>
         <v>0</v>
       </c>
       <c r="AK21" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D22:D1019,M21,J22:J1019,"3+X3")+COUNTIFS(D22:D1019,M21,J22:J1019,"1,3")+COUNTIFS(D22:D1019,M21,J22:J1019,"2,3")+COUNTIFS(D22:D1019,M21,J22:J1019,"1,2,3"))/O21</f>
         <v>0.5</v>
       </c>
       <c r="AL21" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D21:D1019,M21,K21:K1019,"1")/O21</f>
         <v>1</v>
       </c>
       <c r="AM21" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D21:D1019,M21,K21:K1019,"2")/O21</f>
         <v>0</v>
       </c>
       <c r="AN21" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D21:D1019,M21,K21:K1019,"3")/O21</f>
         <v>0</v>
       </c>
       <c r="AO21" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D21:D1019,M21,K21:K1019,"4")/O21</f>
         <v>0</v>
       </c>
     </row>
@@ -7988,114 +7950,114 @@
         <v>35</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D23:D1021,M22)</f>
         <v>1</v>
       </c>
       <c r="P22" s="3">
-        <f t="shared" si="27"/>
+        <f>O22/$M$32</f>
         <v>0.01</v>
       </c>
       <c r="Q22" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P22&gt;0.7,"A",IF(P22&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R22" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F23:F1021,D23:D1021,M22)</f>
         <v>5</v>
       </c>
       <c r="S22" s="1">
-        <f t="shared" si="6"/>
+        <f>R22/O22</f>
         <v>5</v>
       </c>
       <c r="T22" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S22-1)/4)</f>
         <v>0</v>
       </c>
       <c r="U22" s="3">
-        <f t="shared" si="3"/>
+        <f>(P22+T22+Z22)/3</f>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="V22" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D22:D1020,M22,E22:E1020,"1")/O22</f>
         <v>0</v>
       </c>
       <c r="W22" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D22:D1020,M22,E22:E1020,"2")/O22</f>
         <v>0</v>
       </c>
       <c r="X22" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D22:D1020,M22,E22:E1020,"3")/O22</f>
         <v>1</v>
       </c>
       <c r="Y22" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E22:E1020,D22:D1020,M22)/O22</f>
         <v>3</v>
       </c>
       <c r="Z22" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y22-1)/2)</f>
         <v>0</v>
       </c>
       <c r="AA22" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D22:D1020,M22,G22:G1020,"1")/O22</f>
         <v>0</v>
       </c>
       <c r="AB22" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D22:D1020,M22,G22:G1020,"2")/O22</f>
         <v>1</v>
       </c>
       <c r="AC22" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D22:D1020,M22,G22:G1020,"3")/O22</f>
         <v>0</v>
       </c>
       <c r="AD22" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D23:D1020,M22,H23:H1020,"1")+COUNTIFS(D23:D1020,M22,H23:H1020,"1,2"))/O22</f>
         <v>1</v>
       </c>
       <c r="AE22" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D23:D1020,M22,H23:H1020,"2")+COUNTIFS(D23:D1020,M22,H23:H1020,"1,2"))/O22</f>
         <v>1</v>
       </c>
       <c r="AF22" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D23:D1020,M22,I23:I1020,"1")+COUNTIFS(D23:D1020,M22,I23:I1020,"1,2")+COUNTIFS(D23:D1020,M22,I23:I1020,"1,3")+COUNTIFS(D23:D1020,M22,I23:I1020,"1,2,3"))/O22</f>
         <v>0</v>
       </c>
       <c r="AG22" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D23:D1020,M22,I23:I1020,"2")+COUNTIFS(D23:D1020,M22,I23:I1020,"1,2")+COUNTIFS(D23:D1020,M22,I23:I1020,"2,3")+COUNTIFS(D23:D1020,M22,I23:I1020,"1,2,3"))/O22</f>
         <v>1</v>
       </c>
       <c r="AH22" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D23:D1020,M22,I23:I1020,"3")+COUNTIFS(D23:D1020,M22,I23:I1020,"1,3")+COUNTIFS(D23:D1020,M22,I23:I1020,"2,3")+COUNTIFS(D23:D1020,M22,I23:I1020,"1,2,3"))/O22</f>
         <v>1</v>
       </c>
       <c r="AI22" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D23:D1020,M22,J23:J1020,"1")+COUNTIFS(D23:D1020,M22,J23:J1020,"1,2")+COUNTIFS(D23:D1020,M22,J23:J1020,"1,3")+COUNTIFS(D23:D1020,M22,J23:J1020,"1,2,3"))/O22</f>
         <v>1</v>
       </c>
       <c r="AJ22" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D23:D1020,M22,J23:J1020,"2")+COUNTIFS(D23:D1020,M22,J23:J1020,"1,2")+COUNTIFS(D23:D1020,M22,J23:J1020,"2,3")+COUNTIFS(D23:D1020,M22,J23:J1020,"1,2,3"))/O22</f>
         <v>0</v>
       </c>
       <c r="AK22" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D23:D1020,M22,J23:J1020,"3+X3")+COUNTIFS(D23:D1020,M22,J23:J1020,"1,3")+COUNTIFS(D23:D1020,M22,J23:J1020,"2,3")+COUNTIFS(D23:D1020,M22,J23:J1020,"1,2,3"))/O22</f>
         <v>0</v>
       </c>
       <c r="AL22" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D22:D1020,M22,K22:K1020,"1")/O22</f>
         <v>0</v>
       </c>
       <c r="AM22" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D22:D1020,M22,K22:K1020,"2")/O22</f>
         <v>1</v>
       </c>
       <c r="AN22" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D22:D1020,M22,K22:K1020,"3")/O22</f>
         <v>0</v>
       </c>
       <c r="AO22" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D22:D1020,M22,K22:K1020,"4")/O22</f>
         <v>0</v>
       </c>
     </row>
@@ -8137,114 +8099,114 @@
         <v>36</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D24:D1022,M23)</f>
         <v>1</v>
       </c>
       <c r="P23" s="3">
-        <f t="shared" si="27"/>
+        <f>O23/$M$32</f>
         <v>0.01</v>
       </c>
       <c r="Q23" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P23&gt;0.7,"A",IF(P23&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R23" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F24:F1022,D24:D1022,M23)</f>
         <v>2</v>
       </c>
       <c r="S23" s="1">
-        <f t="shared" si="6"/>
+        <f>R23/O23</f>
         <v>2</v>
       </c>
       <c r="T23" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S23-1)/4)</f>
         <v>0.75</v>
       </c>
       <c r="U23" s="3">
-        <f t="shared" si="3"/>
+        <f>(P23+T23+Z23)/3</f>
         <v>0.42</v>
       </c>
       <c r="V23" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D23:D1021,M23,E23:E1021,"1")/O23</f>
         <v>0</v>
       </c>
       <c r="W23" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D23:D1021,M23,E23:E1021,"2")/O23</f>
         <v>1</v>
       </c>
       <c r="X23" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D23:D1021,M23,E23:E1021,"3")/O23</f>
         <v>0</v>
       </c>
       <c r="Y23" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E23:E1021,D23:D1021,M23)/O23</f>
         <v>2</v>
       </c>
       <c r="Z23" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y23-1)/2)</f>
         <v>0.5</v>
       </c>
       <c r="AA23" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D23:D1021,M23,G23:G1021,"1")/O23</f>
         <v>1</v>
       </c>
       <c r="AB23" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D23:D1021,M23,G23:G1021,"2")/O23</f>
         <v>0</v>
       </c>
       <c r="AC23" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D23:D1021,M23,G23:G1021,"3")/O23</f>
         <v>0</v>
       </c>
       <c r="AD23" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D24:D1021,M23,H24:H1021,"1")+COUNTIFS(D24:D1021,M23,H24:H1021,"1,2"))/O23</f>
         <v>1</v>
       </c>
       <c r="AE23" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D24:D1021,M23,H24:H1021,"2")+COUNTIFS(D24:D1021,M23,H24:H1021,"1,2"))/O23</f>
         <v>0</v>
       </c>
       <c r="AF23" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D24:D1021,M23,I24:I1021,"1")+COUNTIFS(D24:D1021,M23,I24:I1021,"1,2")+COUNTIFS(D24:D1021,M23,I24:I1021,"1,3")+COUNTIFS(D24:D1021,M23,I24:I1021,"1,2,3"))/O23</f>
         <v>0</v>
       </c>
       <c r="AG23" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D24:D1021,M23,I24:I1021,"2")+COUNTIFS(D24:D1021,M23,I24:I1021,"1,2")+COUNTIFS(D24:D1021,M23,I24:I1021,"2,3")+COUNTIFS(D24:D1021,M23,I24:I1021,"1,2,3"))/O23</f>
         <v>1</v>
       </c>
       <c r="AH23" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D24:D1021,M23,I24:I1021,"3")+COUNTIFS(D24:D1021,M23,I24:I1021,"1,3")+COUNTIFS(D24:D1021,M23,I24:I1021,"2,3")+COUNTIFS(D24:D1021,M23,I24:I1021,"1,2,3"))/O23</f>
         <v>0</v>
       </c>
       <c r="AI23" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D24:D1021,M23,J24:J1021,"1")+COUNTIFS(D24:D1021,M23,J24:J1021,"1,2")+COUNTIFS(D24:D1021,M23,J24:J1021,"1,3")+COUNTIFS(D24:D1021,M23,J24:J1021,"1,2,3"))/O23</f>
         <v>1</v>
       </c>
       <c r="AJ23" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D24:D1021,M23,J24:J1021,"2")+COUNTIFS(D24:D1021,M23,J24:J1021,"1,2")+COUNTIFS(D24:D1021,M23,J24:J1021,"2,3")+COUNTIFS(D24:D1021,M23,J24:J1021,"1,2,3"))/O23</f>
         <v>0</v>
       </c>
       <c r="AK23" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D24:D1021,M23,J24:J1021,"3+X3")+COUNTIFS(D24:D1021,M23,J24:J1021,"1,3")+COUNTIFS(D24:D1021,M23,J24:J1021,"2,3")+COUNTIFS(D24:D1021,M23,J24:J1021,"1,2,3"))/O23</f>
         <v>0</v>
       </c>
       <c r="AL23" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D23:D1021,M23,K23:K1021,"1")/O23</f>
         <v>1</v>
       </c>
       <c r="AM23" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D23:D1021,M23,K23:K1021,"2")/O23</f>
         <v>0</v>
       </c>
       <c r="AN23" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D23:D1021,M23,K23:K1021,"3")/O23</f>
         <v>0</v>
       </c>
       <c r="AO23" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D23:D1021,M23,K23:K1021,"4")/O23</f>
         <v>0</v>
       </c>
     </row>
@@ -8286,114 +8248,114 @@
         <v>37</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D25:D1023,M24)</f>
         <v>1</v>
       </c>
       <c r="P24" s="3">
-        <f t="shared" si="27"/>
+        <f>O24/$M$32</f>
         <v>0.01</v>
       </c>
       <c r="Q24" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P24&gt;0.7,"A",IF(P24&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R24" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F25:F1023,D25:D1023,M24)</f>
         <v>2</v>
       </c>
       <c r="S24" s="1">
-        <f t="shared" si="6"/>
+        <f>R24/O24</f>
         <v>2</v>
       </c>
       <c r="T24" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S24-1)/4)</f>
         <v>0.75</v>
       </c>
       <c r="U24" s="3">
-        <f t="shared" si="3"/>
+        <f>(P24+T24+Z24)/3</f>
         <v>0.42</v>
       </c>
       <c r="V24" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D24:D1022,M24,E24:E1022,"1")/O24</f>
         <v>0</v>
       </c>
       <c r="W24" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D24:D1022,M24,E24:E1022,"2")/O24</f>
         <v>1</v>
       </c>
       <c r="X24" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D24:D1022,M24,E24:E1022,"3")/O24</f>
         <v>0</v>
       </c>
       <c r="Y24" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E24:E1022,D24:D1022,M24)/O24</f>
         <v>2</v>
       </c>
       <c r="Z24" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y24-1)/2)</f>
         <v>0.5</v>
       </c>
       <c r="AA24" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D24:D1022,M24,G24:G1022,"1")/O24</f>
         <v>0</v>
       </c>
       <c r="AB24" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D24:D1022,M24,G24:G1022,"2")/O24</f>
         <v>0</v>
       </c>
       <c r="AC24" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D24:D1022,M24,G24:G1022,"3")/O24</f>
         <v>1</v>
       </c>
       <c r="AD24" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D25:D1022,M24,H25:H1022,"1")+COUNTIFS(D25:D1022,M24,H25:H1022,"1,2"))/O24</f>
         <v>1</v>
       </c>
       <c r="AE24" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D25:D1022,M24,H25:H1022,"2")+COUNTIFS(D25:D1022,M24,H25:H1022,"1,2"))/O24</f>
         <v>1</v>
       </c>
       <c r="AF24" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D25:D1022,M24,I25:I1022,"1")+COUNTIFS(D25:D1022,M24,I25:I1022,"1,2")+COUNTIFS(D25:D1022,M24,I25:I1022,"1,3")+COUNTIFS(D25:D1022,M24,I25:I1022,"1,2,3"))/O24</f>
         <v>0</v>
       </c>
       <c r="AG24" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D25:D1022,M24,I25:I1022,"2")+COUNTIFS(D25:D1022,M24,I25:I1022,"1,2")+COUNTIFS(D25:D1022,M24,I25:I1022,"2,3")+COUNTIFS(D25:D1022,M24,I25:I1022,"1,2,3"))/O24</f>
         <v>1</v>
       </c>
       <c r="AH24" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D25:D1022,M24,I25:I1022,"3")+COUNTIFS(D25:D1022,M24,I25:I1022,"1,3")+COUNTIFS(D25:D1022,M24,I25:I1022,"2,3")+COUNTIFS(D25:D1022,M24,I25:I1022,"1,2,3"))/O24</f>
         <v>1</v>
       </c>
       <c r="AI24" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D25:D1022,M24,J25:J1022,"1")+COUNTIFS(D25:D1022,M24,J25:J1022,"1,2")+COUNTIFS(D25:D1022,M24,J25:J1022,"1,3")+COUNTIFS(D25:D1022,M24,J25:J1022,"1,2,3"))/O24</f>
         <v>0</v>
       </c>
       <c r="AJ24" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D25:D1022,M24,J25:J1022,"2")+COUNTIFS(D25:D1022,M24,J25:J1022,"1,2")+COUNTIFS(D25:D1022,M24,J25:J1022,"2,3")+COUNTIFS(D25:D1022,M24,J25:J1022,"1,2,3"))/O24</f>
         <v>0</v>
       </c>
       <c r="AK24" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D25:D1022,M24,J25:J1022,"3+X3")+COUNTIFS(D25:D1022,M24,J25:J1022,"1,3")+COUNTIFS(D25:D1022,M24,J25:J1022,"2,3")+COUNTIFS(D25:D1022,M24,J25:J1022,"1,2,3"))/O24</f>
         <v>0</v>
       </c>
       <c r="AL24" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D24:D1022,M24,K24:K1022,"1")/O24</f>
         <v>0</v>
       </c>
       <c r="AM24" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D24:D1022,M24,K24:K1022,"2")/O24</f>
         <v>1</v>
       </c>
       <c r="AN24" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D24:D1022,M24,K24:K1022,"3")/O24</f>
         <v>0</v>
       </c>
       <c r="AO24" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D24:D1022,M24,K24:K1022,"4")/O24</f>
         <v>0</v>
       </c>
     </row>
@@ -8438,111 +8400,111 @@
         <v>83</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D26:D1024,M25)</f>
         <v>1</v>
       </c>
       <c r="P25" s="3">
-        <f t="shared" si="27"/>
+        <f>O25/$M$32</f>
         <v>0.01</v>
       </c>
       <c r="Q25" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P25&gt;0.7,"A",IF(P25&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R25" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F26:F1024,D26:D1024,M25)</f>
         <v>1</v>
       </c>
       <c r="S25" s="1">
-        <f t="shared" si="6"/>
+        <f>R25/O25</f>
         <v>1</v>
       </c>
       <c r="T25" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S25-1)/4)</f>
         <v>1</v>
       </c>
       <c r="U25" s="3">
-        <f t="shared" si="3"/>
+        <f>(P25+T25+Z25)/3</f>
         <v>0.66999999999999993</v>
       </c>
       <c r="V25" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D25:D1023,M25,E25:E1023,"1")/O25</f>
         <v>1</v>
       </c>
       <c r="W25" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D25:D1023,M25,E25:E1023,"2")/O25</f>
         <v>0</v>
       </c>
       <c r="X25" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D25:D1023,M25,E25:E1023,"3")/O25</f>
         <v>0</v>
       </c>
       <c r="Y25" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E25:E1023,D25:D1023,M25)/O25</f>
         <v>1</v>
       </c>
       <c r="Z25" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y25-1)/2)</f>
         <v>1</v>
       </c>
       <c r="AA25" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D25:D1023,M25,G25:G1023,"1")/O25</f>
         <v>0</v>
       </c>
       <c r="AB25" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D25:D1023,M25,G25:G1023,"2")/O25</f>
         <v>0</v>
       </c>
       <c r="AC25" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D25:D1023,M25,G25:G1023,"3")/O25</f>
         <v>1</v>
       </c>
       <c r="AD25" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D26:D1023,M25,H26:H1023,"1")+COUNTIFS(D26:D1023,M25,H26:H1023,"1,2"))/O25</f>
         <v>1</v>
       </c>
       <c r="AE25" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D26:D1023,M25,H26:H1023,"2")+COUNTIFS(D26:D1023,M25,H26:H1023,"1,2"))/O25</f>
         <v>0</v>
       </c>
       <c r="AF25" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D26:D1023,M25,I26:I1023,"1")+COUNTIFS(D26:D1023,M25,I26:I1023,"1,2")+COUNTIFS(D26:D1023,M25,I26:I1023,"1,3")+COUNTIFS(D26:D1023,M25,I26:I1023,"1,2,3"))/O25</f>
         <v>0</v>
       </c>
       <c r="AG25" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D26:D1023,M25,I26:I1023,"2")+COUNTIFS(D26:D1023,M25,I26:I1023,"1,2")+COUNTIFS(D26:D1023,M25,I26:I1023,"2,3")+COUNTIFS(D26:D1023,M25,I26:I1023,"1,2,3"))/O25</f>
         <v>1</v>
       </c>
       <c r="AH25" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D26:D1023,M25,I26:I1023,"3")+COUNTIFS(D26:D1023,M25,I26:I1023,"1,3")+COUNTIFS(D26:D1023,M25,I26:I1023,"2,3")+COUNTIFS(D26:D1023,M25,I26:I1023,"1,2,3"))/O25</f>
         <v>0</v>
       </c>
       <c r="AI25" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D26:D1023,M25,J26:J1023,"1")+COUNTIFS(D26:D1023,M25,J26:J1023,"1,2")+COUNTIFS(D26:D1023,M25,J26:J1023,"1,3")+COUNTIFS(D26:D1023,M25,J26:J1023,"1,2,3"))/O25</f>
         <v>0</v>
       </c>
       <c r="AJ25" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D26:D1023,M25,J26:J1023,"2")+COUNTIFS(D26:D1023,M25,J26:J1023,"1,2")+COUNTIFS(D26:D1023,M25,J26:J1023,"2,3")+COUNTIFS(D26:D1023,M25,J26:J1023,"1,2,3"))/O25</f>
         <v>1</v>
       </c>
       <c r="AK25" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D26:D1023,M25,J26:J1023,"3+X3")+COUNTIFS(D26:D1023,M25,J26:J1023,"1,3")+COUNTIFS(D26:D1023,M25,J26:J1023,"2,3")+COUNTIFS(D26:D1023,M25,J26:J1023,"1,2,3"))/O25</f>
         <v>1</v>
       </c>
       <c r="AL25" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D25:D1023,M25,K25:K1023,"1")/O25</f>
         <v>1</v>
       </c>
       <c r="AM25" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D25:D1023,M25,K25:K1023,"2")/O25</f>
         <v>0</v>
       </c>
       <c r="AN25" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D25:D1023,M25,K25:K1023,"3")/O25</f>
         <v>0</v>
       </c>
       <c r="AO25" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D25:D1023,M25,K25:K1023,"4")/O25</f>
         <v>0</v>
       </c>
     </row>
@@ -8584,114 +8546,114 @@
         <v>72</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="7"/>
+        <f>COUNTIF(D27:D1025,M26)</f>
         <v>1</v>
       </c>
       <c r="P26" s="3">
-        <f t="shared" si="27"/>
+        <f>O26/$M$32</f>
         <v>0.01</v>
       </c>
       <c r="Q26" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(P26&gt;0.7,"A",IF(P26&gt;0.1,"B","C"))</f>
         <v>C</v>
       </c>
       <c r="R26" s="1">
-        <f t="shared" si="8"/>
+        <f>SUMIFS(F27:F1025,D27:D1025,M26)</f>
         <v>2</v>
       </c>
       <c r="S26" s="1">
-        <f t="shared" si="6"/>
+        <f>R26/O26</f>
         <v>2</v>
       </c>
       <c r="T26" s="3">
-        <f t="shared" si="2"/>
+        <f>1-((S26-1)/4)</f>
         <v>0.75</v>
       </c>
       <c r="U26" s="3">
-        <f t="shared" si="3"/>
+        <f>(P26+T26+Z26)/3</f>
         <v>0.25333333333333335</v>
       </c>
       <c r="V26" s="9">
-        <f t="shared" si="9"/>
+        <f>COUNTIFS(D26:D1024,M26,E26:E1024,"1")/O26</f>
         <v>0</v>
       </c>
       <c r="W26" s="3">
-        <f t="shared" si="10"/>
+        <f>COUNTIFS(D26:D1024,M26,E26:E1024,"2")/O26</f>
         <v>0</v>
       </c>
       <c r="X26" s="3">
-        <f t="shared" si="11"/>
+        <f>COUNTIFS(D26:D1024,M26,E26:E1024,"3")/O26</f>
         <v>1</v>
       </c>
       <c r="Y26" s="12">
-        <f t="shared" si="4"/>
+        <f>SUMIFS(E26:E1024,D26:D1024,M26)/O26</f>
         <v>3</v>
       </c>
       <c r="Z26" s="3">
-        <f t="shared" si="5"/>
+        <f>1-((Y26-1)/2)</f>
         <v>0</v>
       </c>
       <c r="AA26" s="9">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS(D26:D1024,M26,G26:G1024,"1")/O26</f>
         <v>0</v>
       </c>
       <c r="AB26" s="3">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS(D26:D1024,M26,G26:G1024,"2")/O26</f>
         <v>0</v>
       </c>
       <c r="AC26" s="3">
-        <f t="shared" si="14"/>
+        <f>COUNTIFS(D26:D1024,M26,G26:G1024,"3")/O26</f>
         <v>1</v>
       </c>
       <c r="AD26" s="9">
-        <f t="shared" si="15"/>
+        <f>(COUNTIFS(D27:D1024,M26,H27:H1024,"1")+COUNTIFS(D27:D1024,M26,H27:H1024,"1,2"))/O26</f>
         <v>0</v>
       </c>
       <c r="AE26" s="3">
-        <f t="shared" si="16"/>
+        <f>(COUNTIFS(D27:D1024,M26,H27:H1024,"2")+COUNTIFS(D27:D1024,M26,H27:H1024,"1,2"))/O26</f>
         <v>1</v>
       </c>
       <c r="AF26" s="9">
-        <f t="shared" si="17"/>
+        <f>(COUNTIFS(D27:D1024,M26,I27:I1024,"1")+COUNTIFS(D27:D1024,M26,I27:I1024,"1,2")+COUNTIFS(D27:D1024,M26,I27:I1024,"1,3")+COUNTIFS(D27:D1024,M26,I27:I1024,"1,2,3"))/O26</f>
         <v>0</v>
       </c>
       <c r="AG26" s="3">
-        <f t="shared" si="18"/>
+        <f>(COUNTIFS(D27:D1024,M26,I27:I1024,"2")+COUNTIFS(D27:D1024,M26,I27:I1024,"1,2")+COUNTIFS(D27:D1024,M26,I27:I1024,"2,3")+COUNTIFS(D27:D1024,M26,I27:I1024,"1,2,3"))/O26</f>
         <v>0</v>
       </c>
       <c r="AH26" s="3">
-        <f t="shared" si="19"/>
+        <f>(COUNTIFS(D27:D1024,M26,I27:I1024,"3")+COUNTIFS(D27:D1024,M26,I27:I1024,"1,3")+COUNTIFS(D27:D1024,M26,I27:I1024,"2,3")+COUNTIFS(D27:D1024,M26,I27:I1024,"1,2,3"))/O26</f>
         <v>1</v>
       </c>
       <c r="AI26" s="9">
-        <f t="shared" si="20"/>
+        <f>(COUNTIFS(D27:D1024,M26,J27:J1024,"1")+COUNTIFS(D27:D1024,M26,J27:J1024,"1,2")+COUNTIFS(D27:D1024,M26,J27:J1024,"1,3")+COUNTIFS(D27:D1024,M26,J27:J1024,"1,2,3"))/O26</f>
         <v>0</v>
       </c>
       <c r="AJ26" s="3">
-        <f t="shared" si="21"/>
+        <f>(COUNTIFS(D27:D1024,M26,J27:J1024,"2")+COUNTIFS(D27:D1024,M26,J27:J1024,"1,2")+COUNTIFS(D27:D1024,M26,J27:J1024,"2,3")+COUNTIFS(D27:D1024,M26,J27:J1024,"1,2,3"))/O26</f>
         <v>0</v>
       </c>
       <c r="AK26" s="3">
-        <f t="shared" si="22"/>
+        <f>(COUNTIFS(D27:D1024,M26,J27:J1024,"3+X3")+COUNTIFS(D27:D1024,M26,J27:J1024,"1,3")+COUNTIFS(D27:D1024,M26,J27:J1024,"2,3")+COUNTIFS(D27:D1024,M26,J27:J1024,"1,2,3"))/O26</f>
         <v>0</v>
       </c>
       <c r="AL26" s="9">
-        <f t="shared" si="23"/>
+        <f>COUNTIFS(D26:D1024,M26,K26:K1024,"1")/O26</f>
         <v>1</v>
       </c>
       <c r="AM26" s="3">
-        <f t="shared" si="24"/>
+        <f>COUNTIFS(D26:D1024,M26,K26:K1024,"2")/O26</f>
         <v>0</v>
       </c>
       <c r="AN26" s="3">
-        <f t="shared" si="25"/>
+        <f>COUNTIFS(D26:D1024,M26,K26:K1024,"3")/O26</f>
         <v>0</v>
       </c>
       <c r="AO26" s="3">
-        <f t="shared" si="26"/>
+        <f>COUNTIFS(D26:D1024,M26,K26:K1024,"4")/O26</f>
         <v>0</v>
       </c>
     </row>
@@ -8771,7 +8733,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O28" s="1">
         <f>SUM(O3:O26)</f>
@@ -8846,15 +8808,15 @@
         <v>0.54766355140186918</v>
       </c>
       <c r="AM29" s="9">
-        <f t="shared" ref="AM29:AO29" si="28">AM28/535</f>
+        <f t="shared" ref="AM29:AO29" si="6">AM28/535</f>
         <v>0.23177570093457944</v>
       </c>
       <c r="AN29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="6"/>
         <v>4.2990654205607479E-2</v>
       </c>
       <c r="AO29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="6"/>
         <v>0.17570093457943925</v>
       </c>
     </row>
@@ -8931,13 +8893,13 @@
         <v>33</v>
       </c>
       <c r="N31" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="O31" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="O31" s="20" t="s">
+      <c r="P31" s="20" t="s">
         <v>92</v>
-      </c>
-      <c r="P31" s="20" t="s">
-        <v>93</v>
       </c>
       <c r="Q31"/>
       <c r="R31"/>
@@ -8949,16 +8911,16 @@
         <v>82</v>
       </c>
       <c r="V31" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="W31" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="X31" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y31" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="W31" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="X31" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y31" s="18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:41" ht="17.25" thickTop="1" thickBot="1">
@@ -9011,7 +8973,7 @@
       <c r="Q32"/>
       <c r="R32"/>
       <c r="S32" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T32" s="18">
         <f>SUMIFS(O3:O26,N3:N26,T31)</f>
@@ -9073,7 +9035,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T33" s="19">
         <f>T32/O28</f>
@@ -9553,15 +9515,15 @@
         <v>2</v>
       </c>
       <c r="S44" s="1">
-        <f t="shared" ref="S44:S51" si="29">SUMIFS(N44:N1002,O44:O1002,R44)</f>
+        <f t="shared" ref="S44:S51" si="7">SUMIFS(N44:N1002,O44:O1002,R44)</f>
         <v>64</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" ref="T44:T51" si="30">COUNTIF(O44:O1002,R44)</f>
+        <f t="shared" ref="T44:T51" si="8">COUNTIF(O44:O1002,R44)</f>
         <v>14</v>
       </c>
       <c r="U44" s="1">
-        <f t="shared" ref="U44:U49" si="31">S44/T44</f>
+        <f t="shared" ref="U44:U49" si="9">S44/T44</f>
         <v>4.5714285714285712</v>
       </c>
     </row>
@@ -9616,15 +9578,15 @@
         <v>3</v>
       </c>
       <c r="S45" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
       <c r="T45" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="U45" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="9"/>
         <v>6.117647058823529</v>
       </c>
     </row>
@@ -9666,7 +9628,7 @@
         <v>4</v>
       </c>
       <c r="N46" s="1">
-        <f t="shared" ref="N46:N50" si="32">COUNTIF(A4:A1001,M46)</f>
+        <f t="shared" ref="N46:N50" si="10">COUNTIF(A4:A1001,M46)</f>
         <v>4</v>
       </c>
       <c r="O46" s="1">
@@ -9679,15 +9641,15 @@
         <v>4</v>
       </c>
       <c r="S46" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="7"/>
         <v>124</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="U46" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="9"/>
         <v>5.6363636363636367</v>
       </c>
     </row>
@@ -9729,7 +9691,7 @@
         <v>5</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="O47" s="1">
@@ -9742,15 +9704,15 @@
         <v>5</v>
       </c>
       <c r="S47" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="7"/>
         <v>112</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="U47" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="9"/>
         <v>7.4666666666666668</v>
       </c>
     </row>
@@ -9792,7 +9754,7 @@
         <v>6</v>
       </c>
       <c r="N48" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="O48" s="1">
@@ -9805,15 +9767,15 @@
         <v>6</v>
       </c>
       <c r="S48" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9855,7 +9817,7 @@
         <v>7</v>
       </c>
       <c r="N49" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="O49" s="1">
@@ -9868,15 +9830,15 @@
         <v>7</v>
       </c>
       <c r="S49" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
     </row>
@@ -9918,7 +9880,7 @@
         <v>8</v>
       </c>
       <c r="N50" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="O50" s="1">
@@ -9931,11 +9893,11 @@
         <v>8</v>
       </c>
       <c r="S50" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U50" s="1">
@@ -9993,11 +9955,11 @@
         <v>9</v>
       </c>
       <c r="S51" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U51" s="1">
@@ -10042,7 +10004,7 @@
         <v>10</v>
       </c>
       <c r="N52" s="1">
-        <f t="shared" ref="N52:N115" si="33">COUNTIF(A10:A1007,M52)</f>
+        <f t="shared" ref="N52:N115" si="11">COUNTIF(A10:A1007,M52)</f>
         <v>1</v>
       </c>
       <c r="O52" s="1">
@@ -10090,7 +10052,7 @@
         <v>11</v>
       </c>
       <c r="N53" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O53" s="1">
@@ -10138,7 +10100,7 @@
         <v>12</v>
       </c>
       <c r="N54" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O54" s="1">
@@ -10186,7 +10148,7 @@
         <v>13</v>
       </c>
       <c r="N55" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O55" s="1">
@@ -10234,7 +10196,7 @@
         <v>14</v>
       </c>
       <c r="N56" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O56" s="1">
@@ -10282,7 +10244,7 @@
         <v>15</v>
       </c>
       <c r="N57" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O57" s="1">
@@ -10330,7 +10292,7 @@
         <v>16</v>
       </c>
       <c r="N58" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O58" s="1">
@@ -10378,7 +10340,7 @@
         <v>17</v>
       </c>
       <c r="N59" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O59" s="1">
@@ -10426,7 +10388,7 @@
         <v>18</v>
       </c>
       <c r="N60" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O60" s="1">
@@ -10475,7 +10437,7 @@
         <v>19</v>
       </c>
       <c r="N61" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O61" s="1">
@@ -10523,7 +10485,7 @@
         <v>20</v>
       </c>
       <c r="N62" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O62" s="1">
@@ -10571,7 +10533,7 @@
         <v>21</v>
       </c>
       <c r="N63" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O63" s="1">
@@ -10619,7 +10581,7 @@
         <v>22</v>
       </c>
       <c r="N64" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="O64" s="1">
@@ -10667,7 +10629,7 @@
         <v>23</v>
       </c>
       <c r="N65" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O65" s="1">
@@ -10715,7 +10677,7 @@
         <v>24</v>
       </c>
       <c r="N66" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O66" s="1">
@@ -10763,7 +10725,7 @@
         <v>25</v>
       </c>
       <c r="N67" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O67" s="1">
@@ -10811,7 +10773,7 @@
         <v>26</v>
       </c>
       <c r="N68" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O68" s="1">
@@ -10859,7 +10821,7 @@
         <v>27</v>
       </c>
       <c r="N69" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O69" s="1">
@@ -10907,7 +10869,7 @@
         <v>28</v>
       </c>
       <c r="N70" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O70" s="1">
@@ -10955,7 +10917,7 @@
         <v>29</v>
       </c>
       <c r="N71" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O71" s="1">
@@ -11003,7 +10965,7 @@
         <v>30</v>
       </c>
       <c r="N72" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O72" s="1">
@@ -11051,7 +11013,7 @@
         <v>31</v>
       </c>
       <c r="N73" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O73" s="1">
@@ -11099,7 +11061,7 @@
         <v>32</v>
       </c>
       <c r="N74" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O74" s="1">
@@ -11147,7 +11109,7 @@
         <v>33</v>
       </c>
       <c r="N75" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O75" s="1">
@@ -11195,7 +11157,7 @@
         <v>34</v>
       </c>
       <c r="N76" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O76" s="1">
@@ -11243,7 +11205,7 @@
         <v>35</v>
       </c>
       <c r="N77" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="O77" s="1">
@@ -11291,7 +11253,7 @@
         <v>36</v>
       </c>
       <c r="N78" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O78" s="1">
@@ -11339,7 +11301,7 @@
         <v>37</v>
       </c>
       <c r="N79" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="O79" s="1">
@@ -11387,7 +11349,7 @@
         <v>38</v>
       </c>
       <c r="N80" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O80" s="1">
@@ -11435,7 +11397,7 @@
         <v>39</v>
       </c>
       <c r="N81" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O81" s="1">
@@ -11483,7 +11445,7 @@
         <v>40</v>
       </c>
       <c r="N82" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="O82" s="1">
@@ -11531,7 +11493,7 @@
         <v>41</v>
       </c>
       <c r="N83" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O83" s="1">
@@ -11579,7 +11541,7 @@
         <v>42</v>
       </c>
       <c r="N84" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O84" s="1">
@@ -11627,7 +11589,7 @@
         <v>43</v>
       </c>
       <c r="N85" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O85" s="1">
@@ -11675,7 +11637,7 @@
         <v>44</v>
       </c>
       <c r="N86" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O86" s="1">
@@ -11723,7 +11685,7 @@
         <v>45</v>
       </c>
       <c r="N87" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O87" s="1">
@@ -11771,7 +11733,7 @@
         <v>46</v>
       </c>
       <c r="N88" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O88" s="1">
@@ -11819,7 +11781,7 @@
         <v>47</v>
       </c>
       <c r="N89" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O89" s="1">
@@ -11867,7 +11829,7 @@
         <v>48</v>
       </c>
       <c r="N90" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O90" s="1">
@@ -11915,7 +11877,7 @@
         <v>49</v>
       </c>
       <c r="N91" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="O91" s="1">
@@ -11963,7 +11925,7 @@
         <v>50</v>
       </c>
       <c r="N92" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O92" s="1">
@@ -12011,7 +11973,7 @@
         <v>51</v>
       </c>
       <c r="N93" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O93" s="1">
@@ -12059,7 +12021,7 @@
         <v>52</v>
       </c>
       <c r="N94" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O94" s="1">
@@ -12107,7 +12069,7 @@
         <v>53</v>
       </c>
       <c r="N95" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O95" s="1">
@@ -12155,7 +12117,7 @@
         <v>54</v>
       </c>
       <c r="N96" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O96" s="1">
@@ -12203,7 +12165,7 @@
         <v>55</v>
       </c>
       <c r="N97" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O97" s="1">
@@ -12251,7 +12213,7 @@
         <v>56</v>
       </c>
       <c r="N98" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O98" s="1">
@@ -12299,7 +12261,7 @@
         <v>57</v>
       </c>
       <c r="N99" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="O99" s="1">
@@ -12347,7 +12309,7 @@
         <v>58</v>
       </c>
       <c r="N100" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O100" s="1">
@@ -12395,7 +12357,7 @@
         <v>59</v>
       </c>
       <c r="N101" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="O101" s="1">
@@ -12443,7 +12405,7 @@
         <v>60</v>
       </c>
       <c r="N102" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O102" s="1">
@@ -12491,7 +12453,7 @@
         <v>61</v>
       </c>
       <c r="N103" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O103" s="1">
@@ -12539,7 +12501,7 @@
         <v>62</v>
       </c>
       <c r="N104" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O104" s="1">
@@ -12587,7 +12549,7 @@
         <v>63</v>
       </c>
       <c r="N105" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O105" s="1">
@@ -12635,7 +12597,7 @@
         <v>64</v>
       </c>
       <c r="N106" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O106" s="1">
@@ -12683,7 +12645,7 @@
         <v>65</v>
       </c>
       <c r="N107" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O107" s="1">
@@ -12731,7 +12693,7 @@
         <v>66</v>
       </c>
       <c r="N108" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="O108" s="1">
@@ -12779,7 +12741,7 @@
         <v>67</v>
       </c>
       <c r="N109" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="O109" s="1">
@@ -12827,7 +12789,7 @@
         <v>68</v>
       </c>
       <c r="N110" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O110" s="1">
@@ -12875,7 +12837,7 @@
         <v>69</v>
       </c>
       <c r="N111" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="O111" s="1">
@@ -12923,7 +12885,7 @@
         <v>70</v>
       </c>
       <c r="N112" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O112" s="1">
@@ -12971,7 +12933,7 @@
         <v>71</v>
       </c>
       <c r="N113" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O113" s="1">
@@ -13019,7 +12981,7 @@
         <v>72</v>
       </c>
       <c r="N114" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O114" s="1">
@@ -13067,7 +13029,7 @@
         <v>73</v>
       </c>
       <c r="N115" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O115" s="1">
@@ -13115,7 +13077,7 @@
         <v>74</v>
       </c>
       <c r="N116" s="1">
-        <f t="shared" ref="N116:N142" si="34">COUNTIF(A74:A1071,M116)</f>
+        <f t="shared" ref="N116:N142" si="12">COUNTIF(A74:A1071,M116)</f>
         <v>7</v>
       </c>
       <c r="O116" s="1">
@@ -13163,7 +13125,7 @@
         <v>75</v>
       </c>
       <c r="N117" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="O117" s="1">
@@ -13211,7 +13173,7 @@
         <v>76</v>
       </c>
       <c r="N118" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="O118" s="1">
@@ -13259,7 +13221,7 @@
         <v>77</v>
       </c>
       <c r="N119" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O119" s="1">
@@ -13307,7 +13269,7 @@
         <v>78</v>
       </c>
       <c r="N120" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="O120" s="1">
@@ -13355,7 +13317,7 @@
         <v>79</v>
       </c>
       <c r="N121" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="O121" s="1">
@@ -13403,7 +13365,7 @@
         <v>80</v>
       </c>
       <c r="N122" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="O122" s="1">
@@ -13451,7 +13413,7 @@
         <v>81</v>
       </c>
       <c r="N123" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="O123" s="1">
@@ -13499,7 +13461,7 @@
         <v>82</v>
       </c>
       <c r="N124" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="O124" s="1">
@@ -13547,7 +13509,7 @@
         <v>83</v>
       </c>
       <c r="N125" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="O125" s="1">
@@ -13595,7 +13557,7 @@
         <v>84</v>
       </c>
       <c r="N126" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="O126" s="1">
@@ -13643,7 +13605,7 @@
         <v>85</v>
       </c>
       <c r="N127" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="O127" s="1">
@@ -13691,7 +13653,7 @@
         <v>86</v>
       </c>
       <c r="N128" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="O128" s="1">
@@ -13739,7 +13701,7 @@
         <v>87</v>
       </c>
       <c r="N129" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O129" s="1">
@@ -13787,7 +13749,7 @@
         <v>88</v>
       </c>
       <c r="N130" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O130" s="1">
@@ -13835,7 +13797,7 @@
         <v>89</v>
       </c>
       <c r="N131" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="O131" s="1">
@@ -13883,7 +13845,7 @@
         <v>90</v>
       </c>
       <c r="N132" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="O132" s="1">
@@ -13931,7 +13893,7 @@
         <v>91</v>
       </c>
       <c r="N133" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="O133" s="1">
@@ -13979,7 +13941,7 @@
         <v>92</v>
       </c>
       <c r="N134" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="O134" s="1">
@@ -14027,7 +13989,7 @@
         <v>93</v>
       </c>
       <c r="N135" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O135" s="1">
@@ -14075,7 +14037,7 @@
         <v>94</v>
       </c>
       <c r="N136" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O136" s="1">
@@ -14123,7 +14085,7 @@
         <v>95</v>
       </c>
       <c r="N137" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O137" s="1">
@@ -14171,7 +14133,7 @@
         <v>96</v>
       </c>
       <c r="N138" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="O138" s="1">
@@ -14219,7 +14181,7 @@
         <v>97</v>
       </c>
       <c r="N139" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="O139" s="1">
@@ -14267,7 +14229,7 @@
         <v>98</v>
       </c>
       <c r="N140" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O140" s="1">
@@ -14315,7 +14277,7 @@
         <v>99</v>
       </c>
       <c r="N141" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="O141" s="1">
@@ -14363,7 +14325,7 @@
         <v>100</v>
       </c>
       <c r="N142" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="O142" s="1">
@@ -28269,7 +28231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I5:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
@@ -28331,8 +28293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>